<commit_message>
Changes to be committed: 	new file:   .env 	modified:   Broker Analysis.xlsx 	new file:   Top_5_Broker_holdings_2025-06-02.txt 	modified:   nepse.py
</commit_message>
<xml_diff>
--- a/Broker Analysis.xlsx
+++ b/Broker Analysis.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\OneDrive\Desktop\Others\python scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA59A3A7-7332-4AC6-AE6E-51D2694AC3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260A6D65-43AB-4829-A081-6838A3AFEBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2025-05-28" sheetId="4" r:id="rId1"/>
-    <sheet name="2025-05-21" sheetId="3" r:id="rId2"/>
-    <sheet name="2025-05-20" sheetId="2" r:id="rId3"/>
-    <sheet name="2025-05-19" sheetId="1" r:id="rId4"/>
+    <sheet name="2025-06-02" sheetId="5" r:id="rId1"/>
+    <sheet name="2025-05-28" sheetId="4" r:id="rId2"/>
+    <sheet name="2025-05-21" sheetId="3" r:id="rId3"/>
+    <sheet name="2025-05-20" sheetId="2" r:id="rId4"/>
+    <sheet name="2025-05-19" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="2334">
   <si>
     <t>B1</t>
   </si>
@@ -5686,6 +5687,1350 @@
   </si>
   <si>
     <t>SHL/3200/564.80</t>
+  </si>
+  <si>
+    <t>NIFRA/65319/285.41</t>
+  </si>
+  <si>
+    <t>CHDC/7367/2,543.44</t>
+  </si>
+  <si>
+    <t>HIDCL/49346/303.26</t>
+  </si>
+  <si>
+    <t>EBL/22211/645.15</t>
+  </si>
+  <si>
+    <t>HPPL/23540/519.96</t>
+  </si>
+  <si>
+    <t>SHPC/29013/588.99</t>
+  </si>
+  <si>
+    <t>SHIVM/18309/530.16</t>
+  </si>
+  <si>
+    <t>HLI/23291/413.84</t>
+  </si>
+  <si>
+    <t>HIDCL/27253/306.17</t>
+  </si>
+  <si>
+    <t>SARBTM/6986/863.71</t>
+  </si>
+  <si>
+    <t>SARBTM/33696/857.12</t>
+  </si>
+  <si>
+    <t>UPCL/69807/417.01</t>
+  </si>
+  <si>
+    <t>SPDL/32949/384.81</t>
+  </si>
+  <si>
+    <t>MERO/17323/724.02</t>
+  </si>
+  <si>
+    <t>SHIVM/22802/526.38</t>
+  </si>
+  <si>
+    <t>NGPL/78172/382.46</t>
+  </si>
+  <si>
+    <t>HDL/6823/1,236.79</t>
+  </si>
+  <si>
+    <t>HPPL/12517/529.55</t>
+  </si>
+  <si>
+    <t>CHCL/11476/500.79</t>
+  </si>
+  <si>
+    <t>SHPC/9851/590.64</t>
+  </si>
+  <si>
+    <t>NRIC/347058/1,293.49</t>
+  </si>
+  <si>
+    <t>HRL/55463/960.35</t>
+  </si>
+  <si>
+    <t>SHPC/40827/588.49</t>
+  </si>
+  <si>
+    <t>SAHAS/26482/526.03</t>
+  </si>
+  <si>
+    <t>MEN/23175/586.77</t>
+  </si>
+  <si>
+    <t>CHDC/10615/2,536.58</t>
+  </si>
+  <si>
+    <t>RADHI/24393/735.72</t>
+  </si>
+  <si>
+    <t>UPCL/26982/424.45</t>
+  </si>
+  <si>
+    <t>NICA/31367/359.82</t>
+  </si>
+  <si>
+    <t>GHL/37650/259.58</t>
+  </si>
+  <si>
+    <t>LBBL/256772/453.01</t>
+  </si>
+  <si>
+    <t>BPCL/87082/551.32</t>
+  </si>
+  <si>
+    <t>SADBL/79340/429.47</t>
+  </si>
+  <si>
+    <t>LSL/97802/223.70</t>
+  </si>
+  <si>
+    <t>SINDU/16287/834.51</t>
+  </si>
+  <si>
+    <t>GHL/35452/253.28</t>
+  </si>
+  <si>
+    <t>NTC/8110/872.22</t>
+  </si>
+  <si>
+    <t>CIT/2937/1,926.50</t>
+  </si>
+  <si>
+    <t>SHEL/20504/274.75</t>
+  </si>
+  <si>
+    <t>NLICL/7651/624.22</t>
+  </si>
+  <si>
+    <t>BARUN/26959/526.44</t>
+  </si>
+  <si>
+    <t>NABIL/25102/492.80</t>
+  </si>
+  <si>
+    <t>NGPL/23482/386.18</t>
+  </si>
+  <si>
+    <t>BHL/42498/221.37</t>
+  </si>
+  <si>
+    <t>CIT/2984/1,918.06</t>
+  </si>
+  <si>
+    <t>CREST/6446/2,004.36</t>
+  </si>
+  <si>
+    <t>NMIC/4606/2,126.28</t>
+  </si>
+  <si>
+    <t>NIFRA/32435/284.30</t>
+  </si>
+  <si>
+    <t>SHL/14039/569.52</t>
+  </si>
+  <si>
+    <t>SHEL/27256/283.31</t>
+  </si>
+  <si>
+    <t>SAHAS/60533/527.41</t>
+  </si>
+  <si>
+    <t>NGPL/54751/384.33</t>
+  </si>
+  <si>
+    <t>CREST/9806/1,952.69</t>
+  </si>
+  <si>
+    <t>NLG/19619/821.34</t>
+  </si>
+  <si>
+    <t>AHPC/48075/296.22</t>
+  </si>
+  <si>
+    <t>TPC/185153/586.07</t>
+  </si>
+  <si>
+    <t>HURJA/435351/263.37</t>
+  </si>
+  <si>
+    <t>RHPL/179648/396.09</t>
+  </si>
+  <si>
+    <t>NMIC/26995/2,048.99</t>
+  </si>
+  <si>
+    <t>CREST/18999/1,917.87</t>
+  </si>
+  <si>
+    <t>BPCL/304170/497.26</t>
+  </si>
+  <si>
+    <t>SHIVM/136602/531.32</t>
+  </si>
+  <si>
+    <t>SADBL/89897/426.00</t>
+  </si>
+  <si>
+    <t>AHPC/88923/296.55</t>
+  </si>
+  <si>
+    <t>SHPC/26280/597.36</t>
+  </si>
+  <si>
+    <t>LICN/20629/971.67</t>
+  </si>
+  <si>
+    <t>BARUN/31806/542.26</t>
+  </si>
+  <si>
+    <t>UPPER/56151/205.55</t>
+  </si>
+  <si>
+    <t>NLICL/17045/625.06</t>
+  </si>
+  <si>
+    <t>CREST/4473/2,021.97</t>
+  </si>
+  <si>
+    <t>LBBL/77732/467.02</t>
+  </si>
+  <si>
+    <t>BPCL/59344/513.25</t>
+  </si>
+  <si>
+    <t>NADEP/11010/859.69</t>
+  </si>
+  <si>
+    <t>SAPDBL/10015/847.39</t>
+  </si>
+  <si>
+    <t>NLG/9610/812.15</t>
+  </si>
+  <si>
+    <t>LBBL/57110/465.63</t>
+  </si>
+  <si>
+    <t>NGPL/47473/391.23</t>
+  </si>
+  <si>
+    <t>RADHI/24786/741.47</t>
+  </si>
+  <si>
+    <t>NRN/7236/2,037.86</t>
+  </si>
+  <si>
+    <t>SARBTM/16200/851.51</t>
+  </si>
+  <si>
+    <t>NGPL/56076/386.47</t>
+  </si>
+  <si>
+    <t>SADBL/43835/419.71</t>
+  </si>
+  <si>
+    <t>AKJCL/64776/215.04</t>
+  </si>
+  <si>
+    <t>SAHAS/22324/521.05</t>
+  </si>
+  <si>
+    <t>SHIVM/18926/526.19</t>
+  </si>
+  <si>
+    <t>SHIVM/44559/528.75</t>
+  </si>
+  <si>
+    <t>BARUN/36630/530.94</t>
+  </si>
+  <si>
+    <t>SONA/40577/461.59</t>
+  </si>
+  <si>
+    <t>HPPL/26446/531.51</t>
+  </si>
+  <si>
+    <t>PRIN/15472/873.61</t>
+  </si>
+  <si>
+    <t>KBL/197127/215.40</t>
+  </si>
+  <si>
+    <t>HIDCL/108100/305.30</t>
+  </si>
+  <si>
+    <t>SHPC/31727/604.96</t>
+  </si>
+  <si>
+    <t>NICA/27628/358.18</t>
+  </si>
+  <si>
+    <t>SHEL/31350/278.50</t>
+  </si>
+  <si>
+    <t>RADHI/74828/748.05</t>
+  </si>
+  <si>
+    <t>NRN/14628/2,083.26</t>
+  </si>
+  <si>
+    <t>NGPL/57171/379.10</t>
+  </si>
+  <si>
+    <t>MEN/35582/584.10</t>
+  </si>
+  <si>
+    <t>BHL/91904/219.18</t>
+  </si>
+  <si>
+    <t>SAHAS/168324/527.58</t>
+  </si>
+  <si>
+    <t>NGPL/115654/380.95</t>
+  </si>
+  <si>
+    <t>NABBC/16429/1,569.31</t>
+  </si>
+  <si>
+    <t>BPCL/64524/510.03</t>
+  </si>
+  <si>
+    <t>CORBL/14137/2,399.46</t>
+  </si>
+  <si>
+    <t>RADHI/98865/739.21</t>
+  </si>
+  <si>
+    <t>HURJA/69833/267.06</t>
+  </si>
+  <si>
+    <t>UMHL/33264/512.00</t>
+  </si>
+  <si>
+    <t>AHPC/57390/295.96</t>
+  </si>
+  <si>
+    <t>GRDBL/12566/1,256.93</t>
+  </si>
+  <si>
+    <t>CHDC/56963/2,564.98</t>
+  </si>
+  <si>
+    <t>UPCL/289801/429.38</t>
+  </si>
+  <si>
+    <t>HIDCL/129676/305.26</t>
+  </si>
+  <si>
+    <t>SHL/36437/579.97</t>
+  </si>
+  <si>
+    <t>MEN/24473/592.31</t>
+  </si>
+  <si>
+    <t>SBL/441991/291.32</t>
+  </si>
+  <si>
+    <t>RADHI/151931/749.77</t>
+  </si>
+  <si>
+    <t>HRL/56303/970.75</t>
+  </si>
+  <si>
+    <t>EBL/80186/651.58</t>
+  </si>
+  <si>
+    <t>CBBL/37413/902.93</t>
+  </si>
+  <si>
+    <t>API/313148/303.87</t>
+  </si>
+  <si>
+    <t>HIDCL/139097/307.62</t>
+  </si>
+  <si>
+    <t>ALICL/45462/717.95</t>
+  </si>
+  <si>
+    <t>MEN/51991/589.11</t>
+  </si>
+  <si>
+    <t>NIFRA/102699/283.83</t>
+  </si>
+  <si>
+    <t>GBIME/235959/239.38</t>
+  </si>
+  <si>
+    <t>UPCL/69169/418.32</t>
+  </si>
+  <si>
+    <t>NIFRA/91397/281.53</t>
+  </si>
+  <si>
+    <t>HDHPC/102271/213.95</t>
+  </si>
+  <si>
+    <t>SBL/74004/289.10</t>
+  </si>
+  <si>
+    <t>SBI/123826/406.71</t>
+  </si>
+  <si>
+    <t>EBL/37738/625.02</t>
+  </si>
+  <si>
+    <t>SHEL/53119/280.69</t>
+  </si>
+  <si>
+    <t>JBBL/40077/336.71</t>
+  </si>
+  <si>
+    <t>KBL/63336/211.60</t>
+  </si>
+  <si>
+    <t>MEN/11244/584.69</t>
+  </si>
+  <si>
+    <t>SAHAS/9431/522.63</t>
+  </si>
+  <si>
+    <t>SHPC/7192/593.99</t>
+  </si>
+  <si>
+    <t>BHPL/4600/955.74</t>
+  </si>
+  <si>
+    <t>SARBTM/3677/867.84</t>
+  </si>
+  <si>
+    <t>BPCL/216120/520.35</t>
+  </si>
+  <si>
+    <t>SHIVM/71946/527.42</t>
+  </si>
+  <si>
+    <t>CHDC/11910/2,538.76</t>
+  </si>
+  <si>
+    <t>API/63213/308.51</t>
+  </si>
+  <si>
+    <t>SHL/29365/567.95</t>
+  </si>
+  <si>
+    <t>NRN/67015/2,065.24</t>
+  </si>
+  <si>
+    <t>RADHI/203332/709.82</t>
+  </si>
+  <si>
+    <t>UPCL/238055/421.10</t>
+  </si>
+  <si>
+    <t>SHL/30095/564.54</t>
+  </si>
+  <si>
+    <t>SPDL/33437/388.09</t>
+  </si>
+  <si>
+    <t>BPCL/133115/498.98</t>
+  </si>
+  <si>
+    <t>SHEL/74001/280.22</t>
+  </si>
+  <si>
+    <t>MEN/23070/592.97</t>
+  </si>
+  <si>
+    <t>CHDC/4145/2,542.29</t>
+  </si>
+  <si>
+    <t>SANIMA/29662/315.68</t>
+  </si>
+  <si>
+    <t>SAPDBL/90508/942.56</t>
+  </si>
+  <si>
+    <t>GRDBL/26260/1,216.56</t>
+  </si>
+  <si>
+    <t>NMIC/13843/2,093.15</t>
+  </si>
+  <si>
+    <t>SHIVM/42844/528.77</t>
+  </si>
+  <si>
+    <t>SINDU/23468/886.68</t>
+  </si>
+  <si>
+    <t>GBIME/680592/238.97</t>
+  </si>
+  <si>
+    <t>SHPC/144792/597.63</t>
+  </si>
+  <si>
+    <t>RADHI/104184/756.16</t>
+  </si>
+  <si>
+    <t>MERO/107110/743.99</t>
+  </si>
+  <si>
+    <t>AKPL/296489/255.05</t>
+  </si>
+  <si>
+    <t>BPCL/83003/508.52</t>
+  </si>
+  <si>
+    <t>SPIL/29206/822.39</t>
+  </si>
+  <si>
+    <t>SHIVM/31603/532.47</t>
+  </si>
+  <si>
+    <t>USLB/8079/1,942.52</t>
+  </si>
+  <si>
+    <t>MEN/23541/592.25</t>
+  </si>
+  <si>
+    <t>EBL/154647/650.17</t>
+  </si>
+  <si>
+    <t>HRL/66340/969.80</t>
+  </si>
+  <si>
+    <t>PPCL/143356/343.21</t>
+  </si>
+  <si>
+    <t>SHPC/83475/588.10</t>
+  </si>
+  <si>
+    <t>MLBL/115114/394.59</t>
+  </si>
+  <si>
+    <t>SHPC/725020/596.29</t>
+  </si>
+  <si>
+    <t>NLIC/57456/758.71</t>
+  </si>
+  <si>
+    <t>CZBIL/195281/215.77</t>
+  </si>
+  <si>
+    <t>GBIME/170530/224.72</t>
+  </si>
+  <si>
+    <t>CHDC/12336/2,576.19</t>
+  </si>
+  <si>
+    <t>API/52468/303.58</t>
+  </si>
+  <si>
+    <t>HIDCL/31916/296.30</t>
+  </si>
+  <si>
+    <t>AKPL/26987/251.51</t>
+  </si>
+  <si>
+    <t>HPPL/12633/527.82</t>
+  </si>
+  <si>
+    <t>MEN/10608/590.33</t>
+  </si>
+  <si>
+    <t>AHPC/143916/296.17</t>
+  </si>
+  <si>
+    <t>SPDL/34771/385.63</t>
+  </si>
+  <si>
+    <t>CREST/5960/1,992.44</t>
+  </si>
+  <si>
+    <t>SHL/18605/565.44</t>
+  </si>
+  <si>
+    <t>HDHPC/45212/215.95</t>
+  </si>
+  <si>
+    <t>SHL/218873/569.17</t>
+  </si>
+  <si>
+    <t>SHPC/93235/590.13</t>
+  </si>
+  <si>
+    <t>AHPC/99863/299.15</t>
+  </si>
+  <si>
+    <t>NGPL/70343/383.99</t>
+  </si>
+  <si>
+    <t>SHIVM/32440/529.14</t>
+  </si>
+  <si>
+    <t>RADHI/68600/731.25</t>
+  </si>
+  <si>
+    <t>SHPC/75033/596.36</t>
+  </si>
+  <si>
+    <t>MEN/72795/583.55</t>
+  </si>
+  <si>
+    <t>HPPL/50938/531.06</t>
+  </si>
+  <si>
+    <t>NTC/26766/870.49</t>
+  </si>
+  <si>
+    <t>RADHI/367297/743.56</t>
+  </si>
+  <si>
+    <t>SHEL/89281/284.28</t>
+  </si>
+  <si>
+    <t>SHL/42065/577.81</t>
+  </si>
+  <si>
+    <t>HURJA/75680/261.21</t>
+  </si>
+  <si>
+    <t>SPIL/22917/804.87</t>
+  </si>
+  <si>
+    <t>CHDC/19529/2,583.89</t>
+  </si>
+  <si>
+    <t>AHPC/65273/295.80</t>
+  </si>
+  <si>
+    <t>AKPL/74425/251.33</t>
+  </si>
+  <si>
+    <t>API/34813/305.62</t>
+  </si>
+  <si>
+    <t>BHL/35179/219.23</t>
+  </si>
+  <si>
+    <t>CHDC/12187/2,585.73</t>
+  </si>
+  <si>
+    <t>API/27321/307.55</t>
+  </si>
+  <si>
+    <t>RNLI/16884/509.64</t>
+  </si>
+  <si>
+    <t>NIFRA/27439/284.76</t>
+  </si>
+  <si>
+    <t>BHL/35125/218.64</t>
+  </si>
+  <si>
+    <t>NMIC/5395/2,083.82</t>
+  </si>
+  <si>
+    <t>MEN/17502/597.81</t>
+  </si>
+  <si>
+    <t>SHPC/14128/599.41</t>
+  </si>
+  <si>
+    <t>UMHL/17457/513.76</t>
+  </si>
+  <si>
+    <t>SHIVM/14433/526.80</t>
+  </si>
+  <si>
+    <t>STC/12227/5,083.75</t>
+  </si>
+  <si>
+    <t>SADBL/30489/422.60</t>
+  </si>
+  <si>
+    <t>CBBL/12671/856.91</t>
+  </si>
+  <si>
+    <t>BARUN/18854/538.29</t>
+  </si>
+  <si>
+    <t>BHL/36750/219.51</t>
+  </si>
+  <si>
+    <t>GMLI/178320/2,593.04</t>
+  </si>
+  <si>
+    <t>NRIC/248334/1,293.15</t>
+  </si>
+  <si>
+    <t>NMIC/50244/1,966.39</t>
+  </si>
+  <si>
+    <t>NLG/95246/833.88</t>
+  </si>
+  <si>
+    <t>HDL/15979/1,219.34</t>
+  </si>
+  <si>
+    <t>RADHI/88359/759.50</t>
+  </si>
+  <si>
+    <t>NGPL/91333/387.62</t>
+  </si>
+  <si>
+    <t>BEDC/41194/720.52</t>
+  </si>
+  <si>
+    <t>SMHL/30506/945.01</t>
+  </si>
+  <si>
+    <t>MKCL/15413/1,543.56</t>
+  </si>
+  <si>
+    <t>NGPL/167108/383.27</t>
+  </si>
+  <si>
+    <t>RADHI/35344/739.53</t>
+  </si>
+  <si>
+    <t>AHPC/79564/295.49</t>
+  </si>
+  <si>
+    <t>HDHPC/99805/205.51</t>
+  </si>
+  <si>
+    <t>GHL/76837/254.85</t>
+  </si>
+  <si>
+    <t>KBL/1665641/214.43</t>
+  </si>
+  <si>
+    <t>NRN/135675/2,045.73</t>
+  </si>
+  <si>
+    <t>NGPL/309472/383.34</t>
+  </si>
+  <si>
+    <t>AHPC/382718/298.96</t>
+  </si>
+  <si>
+    <t>OHL/106334/950.32</t>
+  </si>
+  <si>
+    <t>SHPC/37707/596.25</t>
+  </si>
+  <si>
+    <t>NGPL/51820/383.46</t>
+  </si>
+  <si>
+    <t>ALICL/27098/712.29</t>
+  </si>
+  <si>
+    <t>NIFRA/49243/286.30</t>
+  </si>
+  <si>
+    <t>API/40760/304.72</t>
+  </si>
+  <si>
+    <t>RADHI/111092/746.67</t>
+  </si>
+  <si>
+    <t>UPCL/128717/421.63</t>
+  </si>
+  <si>
+    <t>SHL/59939/568.81</t>
+  </si>
+  <si>
+    <t>LBBL/50427/474.56</t>
+  </si>
+  <si>
+    <t>SHEL/57272/277.76</t>
+  </si>
+  <si>
+    <t>SHL/29118/567.63</t>
+  </si>
+  <si>
+    <t>CREST/5550/1,948.84</t>
+  </si>
+  <si>
+    <t>NICA/28973/359.78</t>
+  </si>
+  <si>
+    <t>NMIC/3797/2,044.87</t>
+  </si>
+  <si>
+    <t>LSL/31033/226.68</t>
+  </si>
+  <si>
+    <t>UMHL/432982/505.00</t>
+  </si>
+  <si>
+    <t>RIDI/342174/269.65</t>
+  </si>
+  <si>
+    <t>ANLB/4795/5,368.74</t>
+  </si>
+  <si>
+    <t>MKHL/33237/711.22</t>
+  </si>
+  <si>
+    <t>SHIVM/42810/533.25</t>
+  </si>
+  <si>
+    <t>RADHI/28157/744.64</t>
+  </si>
+  <si>
+    <t>SHEL/45245/285.93</t>
+  </si>
+  <si>
+    <t>SHL/23137/561.72</t>
+  </si>
+  <si>
+    <t>KBL/44699/211.49</t>
+  </si>
+  <si>
+    <t>PPCL/27446/345.03</t>
+  </si>
+  <si>
+    <t>BPCL/190494/515.02</t>
+  </si>
+  <si>
+    <t>SHPC/106954/600.19</t>
+  </si>
+  <si>
+    <t>BEDC/61841/741.86</t>
+  </si>
+  <si>
+    <t>NRN/18047/2,064.36</t>
+  </si>
+  <si>
+    <t>LSL/162271/214.43</t>
+  </si>
+  <si>
+    <t>SARBTM/107308/861.55</t>
+  </si>
+  <si>
+    <t>SIKLES/69184/1,089.97</t>
+  </si>
+  <si>
+    <t>PHCL/62679/600.89</t>
+  </si>
+  <si>
+    <t>NGPL/77541/385.27</t>
+  </si>
+  <si>
+    <t>NIFRA/106351/283.27</t>
+  </si>
+  <si>
+    <t>CHDC/42906/2,578.86</t>
+  </si>
+  <si>
+    <t>NRN/22445/2,065.86</t>
+  </si>
+  <si>
+    <t>NGPL/78999/375.83</t>
+  </si>
+  <si>
+    <t>UHEWA/35844/628.93</t>
+  </si>
+  <si>
+    <t>HIDCL/63995/296.92</t>
+  </si>
+  <si>
+    <t>RADHI/103716/763.57</t>
+  </si>
+  <si>
+    <t>HIDCL/93548/303.59</t>
+  </si>
+  <si>
+    <t>SHIVM/25656/535.81</t>
+  </si>
+  <si>
+    <t>HRL/8745/962.49</t>
+  </si>
+  <si>
+    <t>SHEL/22163/283.26</t>
+  </si>
+  <si>
+    <t>NGPL/128228/382.94</t>
+  </si>
+  <si>
+    <t>AHPC/67402/291.91</t>
+  </si>
+  <si>
+    <t>RIDI/63757/263.18</t>
+  </si>
+  <si>
+    <t>HIDCL/50641/305.46</t>
+  </si>
+  <si>
+    <t>SHEL/52362/274.91</t>
+  </si>
+  <si>
+    <t>SHL/91581/563.21</t>
+  </si>
+  <si>
+    <t>API/93937/304.86</t>
+  </si>
+  <si>
+    <t>HIDCL/72944/306.66</t>
+  </si>
+  <si>
+    <t>GLH/67941/278.85</t>
+  </si>
+  <si>
+    <t>SANIMA/57211/310.07</t>
+  </si>
+  <si>
+    <t>BPCL/80250/561.06</t>
+  </si>
+  <si>
+    <t>SHPC/43018/590.77</t>
+  </si>
+  <si>
+    <t>PRVU/79390/217.11</t>
+  </si>
+  <si>
+    <t>CZBIL/43833/220.43</t>
+  </si>
+  <si>
+    <t>NRIC/7204/1,294.90</t>
+  </si>
+  <si>
+    <t>RADHI/80129/732.20</t>
+  </si>
+  <si>
+    <t>LBBL/94136/466.22</t>
+  </si>
+  <si>
+    <t>UPCL/89699/423.26</t>
+  </si>
+  <si>
+    <t>API/99311/306.42</t>
+  </si>
+  <si>
+    <t>SHL/32481/564.71</t>
+  </si>
+  <si>
+    <t>CORBL/53068/2,264.18</t>
+  </si>
+  <si>
+    <t>JOSHI/77941/423.78</t>
+  </si>
+  <si>
+    <t>GRDBL/25554/1,150.47</t>
+  </si>
+  <si>
+    <t>NRN/13368/2,064.29</t>
+  </si>
+  <si>
+    <t>RADHI/35334/743.38</t>
+  </si>
+  <si>
+    <t>LEC/110/226.33</t>
+  </si>
+  <si>
+    <t>GHL/107/253.91</t>
+  </si>
+  <si>
+    <t>SHPC/42995/586.66</t>
+  </si>
+  <si>
+    <t>UPCL/44354/415.37</t>
+  </si>
+  <si>
+    <t>BNHC/26141/518.72</t>
+  </si>
+  <si>
+    <t>MEN/21771/595.54</t>
+  </si>
+  <si>
+    <t>TVCL/19778/502.09</t>
+  </si>
+  <si>
+    <t>NRN/21291/2,079.31</t>
+  </si>
+  <si>
+    <t>API/55832/305.18</t>
+  </si>
+  <si>
+    <t>MFIL/20013/615.98</t>
+  </si>
+  <si>
+    <t>NGPL/29255/382.50</t>
+  </si>
+  <si>
+    <t>BHL/47205/216.30</t>
+  </si>
+  <si>
+    <t>RADHI/28429/730.02</t>
+  </si>
+  <si>
+    <t>MBJC/22878/318.41</t>
+  </si>
+  <si>
+    <t>SHIVM/10652/526.62</t>
+  </si>
+  <si>
+    <t>AKPL/17086/259.92</t>
+  </si>
+  <si>
+    <t>SAHAS/5775/516.29</t>
+  </si>
+  <si>
+    <t>CHDC/36971/2,575.86</t>
+  </si>
+  <si>
+    <t>BPCL/137936/524.03</t>
+  </si>
+  <si>
+    <t>RADHI/75523/753.06</t>
+  </si>
+  <si>
+    <t>NRN/27631/2,062.11</t>
+  </si>
+  <si>
+    <t>SHPC/62526/595.56</t>
+  </si>
+  <si>
+    <t>ALICL/7405/708.65</t>
+  </si>
+  <si>
+    <t>RADHI/6472/753.35</t>
+  </si>
+  <si>
+    <t>NGPL/6435/379.56</t>
+  </si>
+  <si>
+    <t>BHL/3071/220.89</t>
+  </si>
+  <si>
+    <t>MEN/49694/585.29</t>
+  </si>
+  <si>
+    <t>NIFRA/83303/287.60</t>
+  </si>
+  <si>
+    <t>NMLBBL/28882/664.92</t>
+  </si>
+  <si>
+    <t>HRL/18229/974.31</t>
+  </si>
+  <si>
+    <t>USLB/6252/1,845.31</t>
+  </si>
+  <si>
+    <t>NGPL/256795/391.01</t>
+  </si>
+  <si>
+    <t>UPCL/187676/420.91</t>
+  </si>
+  <si>
+    <t>SAHAS/72226/525.24</t>
+  </si>
+  <si>
+    <t>RIDI/118458/271.60</t>
+  </si>
+  <si>
+    <t>HRL/13006/986.06</t>
+  </si>
+  <si>
+    <t>NRN/17069/2,068.56</t>
+  </si>
+  <si>
+    <t>NICA/37299/373.18</t>
+  </si>
+  <si>
+    <t>UMHL/23263/509.84</t>
+  </si>
+  <si>
+    <t>SHIVM/13223/528.47</t>
+  </si>
+  <si>
+    <t>HRL/7128/965.60</t>
+  </si>
+  <si>
+    <t>RADHI/32596/749.22</t>
+  </si>
+  <si>
+    <t>HRL/13500/961.77</t>
+  </si>
+  <si>
+    <t>SAPDBL/10205/787.50</t>
+  </si>
+  <si>
+    <t>AHL/10800/683.54</t>
+  </si>
+  <si>
+    <t>KPCL/13914/524.71</t>
+  </si>
+  <si>
+    <t>HIDCL/103100/301.50</t>
+  </si>
+  <si>
+    <t>SADBL/45521/422.76</t>
+  </si>
+  <si>
+    <t>KSBBL/40011/446.86</t>
+  </si>
+  <si>
+    <t>CZBIL/75311/213.22</t>
+  </si>
+  <si>
+    <t>HDL/12425/1,217.96</t>
+  </si>
+  <si>
+    <t>NGPL/191615/380.91</t>
+  </si>
+  <si>
+    <t>RADHI/51807/749.87</t>
+  </si>
+  <si>
+    <t>SHL/62123/586.22</t>
+  </si>
+  <si>
+    <t>NRN/6661/2,080.05</t>
+  </si>
+  <si>
+    <t>SHEL/43433/282.85</t>
+  </si>
+  <si>
+    <t>CHDC/6027/2,565.95</t>
+  </si>
+  <si>
+    <t>UPCL/37647/413.80</t>
+  </si>
+  <si>
+    <t>NGPL/35527/385.17</t>
+  </si>
+  <si>
+    <t>RADHI/19036/750.45</t>
+  </si>
+  <si>
+    <t>NRIC/8467/1,284.95</t>
+  </si>
+  <si>
+    <t>RADHI/95245/745.41</t>
+  </si>
+  <si>
+    <t>NMIC/4326/2,070.67</t>
+  </si>
+  <si>
+    <t>RIDI/23475/272.81</t>
+  </si>
+  <si>
+    <t>UPCL/15112/415.96</t>
+  </si>
+  <si>
+    <t>HURJA/10405/273.35</t>
+  </si>
+  <si>
+    <t>SAPDBL/31223/902.55</t>
+  </si>
+  <si>
+    <t>GRDBL/16616/1,176.11</t>
+  </si>
+  <si>
+    <t>SHPC/26173/587.63</t>
+  </si>
+  <si>
+    <t>CORBL/5300/2,579.05</t>
+  </si>
+  <si>
+    <t>BARUN/13520/536.32</t>
+  </si>
+  <si>
+    <t>RADHI/35842/739.04</t>
+  </si>
+  <si>
+    <t>GBIME/87044/236.22</t>
+  </si>
+  <si>
+    <t>NGPL/18245/380.38</t>
+  </si>
+  <si>
+    <t>SHIVM/9714/525.78</t>
+  </si>
+  <si>
+    <t>HRL/2732/975.32</t>
+  </si>
+  <si>
+    <t>HBL/93245/230.83</t>
+  </si>
+  <si>
+    <t>BARUN/14335/540.41</t>
+  </si>
+  <si>
+    <t>SHL/10659/573.65</t>
+  </si>
+  <si>
+    <t>CREST/1340/1,908.34</t>
+  </si>
+  <si>
+    <t>AHPC/8126/294.02</t>
+  </si>
+  <si>
+    <t>UPCL/41345/422.32</t>
+  </si>
+  <si>
+    <t>SHPC/22442/585.29</t>
+  </si>
+  <si>
+    <t>NGPL/31054/384.20</t>
+  </si>
+  <si>
+    <t>AKPL/47960/257.01</t>
+  </si>
+  <si>
+    <t>BPCL/21082/520.30</t>
+  </si>
+  <si>
+    <t>HIDCL/177541/300.10</t>
+  </si>
+  <si>
+    <t>SHPC/18803/597.75</t>
+  </si>
+  <si>
+    <t>CHCL/15604/508.62</t>
+  </si>
+  <si>
+    <t>RADHI/7907/738.36</t>
+  </si>
+  <si>
+    <t>NRN/2055/2,075.88</t>
+  </si>
+  <si>
+    <t>BPCL/12763/475.77</t>
+  </si>
+  <si>
+    <t>ICFC/7390/616.11</t>
+  </si>
+  <si>
+    <t>NMIC/1650/1,964.01</t>
+  </si>
+  <si>
+    <t>SHPC/4910/594.00</t>
+  </si>
+  <si>
+    <t>RADHI/187307/755.08</t>
+  </si>
+  <si>
+    <t>MKHL/125115/723.07</t>
+  </si>
+  <si>
+    <t>UPCL/81248/420.23</t>
+  </si>
+  <si>
+    <t>PRIN/31429/869.35</t>
+  </si>
+  <si>
+    <t>BPCL/41042/504.44</t>
+  </si>
+  <si>
+    <t>UPCL/48326/437.10</t>
+  </si>
+  <si>
+    <t>NMIC/3835/2,173.38</t>
+  </si>
+  <si>
+    <t>NMB/26056/240.58</t>
+  </si>
+  <si>
+    <t>NGPL/13447/386.34</t>
+  </si>
+  <si>
+    <t>LBBL/185186/470.28</t>
+  </si>
+  <si>
+    <t>SHL/91064/561.53</t>
+  </si>
+  <si>
+    <t>NICA/108521/366.35</t>
+  </si>
+  <si>
+    <t>NRIC/26673/1,280.54</t>
+  </si>
+  <si>
+    <t>SHPC/44398/599.82</t>
+  </si>
+  <si>
+    <t>SHPC/31395/591.25</t>
+  </si>
+  <si>
+    <t>NRN/6128/2,056.44</t>
+  </si>
+  <si>
+    <t>SADBL/24210/431.15</t>
+  </si>
+  <si>
+    <t>UPCL/17409/427.09</t>
+  </si>
+  <si>
+    <t>NMIC/3043/2,119.01</t>
+  </si>
+  <si>
+    <t>RADHI/37593/728.94</t>
+  </si>
+  <si>
+    <t>NGPL/50748/384.04</t>
+  </si>
+  <si>
+    <t>API/49530/309.63</t>
+  </si>
+  <si>
+    <t>SHPC/22855/577.97</t>
+  </si>
+  <si>
+    <t>AHPC/35404/292.41</t>
+  </si>
+  <si>
+    <t>UNHPL/37014/344.08</t>
+  </si>
+  <si>
+    <t>SHIVM/22968/537.05</t>
+  </si>
+  <si>
+    <t>BPCL/17585/554.77</t>
+  </si>
+  <si>
+    <t>LBBL/15501/467.66</t>
+  </si>
+  <si>
+    <t>SHPC/10442/597.56</t>
+  </si>
+  <si>
+    <t>PHCL/109704/605.37</t>
+  </si>
+  <si>
+    <t>MLBL/37088/389.85</t>
+  </si>
+  <si>
+    <t>RADHI/11862/781.33</t>
+  </si>
+  <si>
+    <t>HDL/8179/1,181.37</t>
+  </si>
+  <si>
+    <t>BGWT/9513/935.01</t>
+  </si>
+  <si>
+    <t>CHDC/5145/2,576.84</t>
+  </si>
+  <si>
+    <t>NGPL/11802/391.05</t>
+  </si>
+  <si>
+    <t>BPCL/6000/582.47</t>
+  </si>
+  <si>
+    <t>LEC/12310/222.38</t>
   </si>
 </sst>
 </file>
@@ -6008,11 +7353,1894 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FC7E8D-1DE3-4DBF-BC92-6657EED87D10}">
+  <dimension ref="A1:F93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1888</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1889</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1891</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1892</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1893</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1894</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1897</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1898</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1899</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1902</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1903</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1904</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1908</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1909</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1911</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1912</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1913</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1914</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1918</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1919</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1923</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1927</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1928</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1929</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1932</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1934</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1939</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1942</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1943</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1949</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1953</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1956</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1957</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1958</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1959</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1961</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1962</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1963</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1964</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1967</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1968</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1969</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1973</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1974</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1983</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1984</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1988</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1989</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1994</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2003</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2009</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2013</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2014</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2018</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2019</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2021</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2022</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2023</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2029</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2038</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2039</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2041</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2042</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2043</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2044</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2049</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2051</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2053</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2054</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2056</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2057</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2058</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2059</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2062</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2063</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2064</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2067</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2071</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2072</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2076</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2077</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2078</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2084</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2087</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2088</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2093</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2097</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2098</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2099</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2103</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2104</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2107</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2108</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2109</v>
+      </c>
+      <c r="F46" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2112</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2114</v>
+      </c>
+      <c r="F47" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2119</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2123</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2124</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>288</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2126</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2127</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2128</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2129</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>300</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2139</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>306</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2141</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2142</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2143</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2144</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>312</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2148</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2153</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2154</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2157</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2158</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>330</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2163</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2164</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>336</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2166</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2167</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2168</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F58" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>342</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2171</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2172</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2173</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F59" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>348</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2177</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2178</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>354</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2181</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2182</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2183</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2184</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>360</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2187</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2188</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2189</v>
+      </c>
+      <c r="F62" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>366</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2192</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2193</v>
+      </c>
+      <c r="E63" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>372</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2196</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2197</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E64" t="s">
+        <v>2199</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>378</v>
+      </c>
+      <c r="B65" t="s">
+        <v>381</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E65" t="s">
+        <v>2201</v>
+      </c>
+      <c r="F65" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2204</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2205</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F66" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>390</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2209</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2210</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2211</v>
+      </c>
+      <c r="F67" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>396</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2213</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2214</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2215</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F68" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2219</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2220</v>
+      </c>
+      <c r="E69" t="s">
+        <v>2221</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>408</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2224</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F70" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>414</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1776</v>
+      </c>
+      <c r="E71" t="s">
+        <v>2226</v>
+      </c>
+      <c r="F71" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>420</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2227</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2229</v>
+      </c>
+      <c r="E72" t="s">
+        <v>2230</v>
+      </c>
+      <c r="F72" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>426</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2233</v>
+      </c>
+      <c r="D73" t="s">
+        <v>2234</v>
+      </c>
+      <c r="E73" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F73" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>432</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2238</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2239</v>
+      </c>
+      <c r="E74" t="s">
+        <v>2240</v>
+      </c>
+      <c r="F74" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>438</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2242</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2243</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E75" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F75" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>444</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2247</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2248</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E76" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F76" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>450</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2252</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D77" t="s">
+        <v>2254</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2255</v>
+      </c>
+      <c r="F77" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>456</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2259</v>
+      </c>
+      <c r="E78" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F78" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>462</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2263</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2264</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2265</v>
+      </c>
+      <c r="F79" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>468</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2267</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D80" t="s">
+        <v>2269</v>
+      </c>
+      <c r="E80" t="s">
+        <v>2270</v>
+      </c>
+      <c r="F80" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>474</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2272</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2273</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E81" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F81" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>480</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2279</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2280</v>
+      </c>
+      <c r="F82" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>486</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2283</v>
+      </c>
+      <c r="D83" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E83" t="s">
+        <v>2285</v>
+      </c>
+      <c r="F83" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>492</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D84" t="s">
+        <v>2289</v>
+      </c>
+      <c r="E84" t="s">
+        <v>2290</v>
+      </c>
+      <c r="F84" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>498</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D85" t="s">
+        <v>2293</v>
+      </c>
+      <c r="E85" t="s">
+        <v>2294</v>
+      </c>
+      <c r="F85" t="s">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>504</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2296</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E86" t="s">
+        <v>2299</v>
+      </c>
+      <c r="F86" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>510</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1854</v>
+      </c>
+      <c r="E87" t="s">
+        <v>2303</v>
+      </c>
+      <c r="F87" t="s">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>516</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2306</v>
+      </c>
+      <c r="D88" t="s">
+        <v>2307</v>
+      </c>
+      <c r="E88" t="s">
+        <v>2308</v>
+      </c>
+      <c r="F88" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>522</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2311</v>
+      </c>
+      <c r="D89" t="s">
+        <v>2312</v>
+      </c>
+      <c r="E89" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F89" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>528</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D90" t="s">
+        <v>2317</v>
+      </c>
+      <c r="E90" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F90" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>534</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D91" t="s">
+        <v>2322</v>
+      </c>
+      <c r="E91" t="s">
+        <v>2323</v>
+      </c>
+      <c r="F91" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>540</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2327</v>
+      </c>
+      <c r="E92" t="s">
+        <v>2328</v>
+      </c>
+      <c r="F92" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>546</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2330</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2331</v>
+      </c>
+      <c r="D93" t="s">
+        <v>2332</v>
+      </c>
+      <c r="E93" t="s">
+        <v>2333</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEF453-2C93-48DA-92A9-F02917F02C21}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7889,7 +11117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3009EEF-D0A3-4418-BB02-D308992E6389}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -9769,7 +12997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62503B16-5D5E-43EB-8EDC-28C65E9BFBAD}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -11649,7 +14877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F93"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Broker Analysis.xlsx 	new file:   Top_5_Broker_holdings_2025-06-03.txt 	modified:   nepse.py
</commit_message>
<xml_diff>
--- a/Broker Analysis.xlsx
+++ b/Broker Analysis.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\OneDrive\Desktop\Others\python scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260A6D65-43AB-4829-A081-6838A3AFEBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E106B-0916-434A-8C6D-13A2A4388BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2025-06-02" sheetId="5" r:id="rId1"/>
-    <sheet name="2025-05-28" sheetId="4" r:id="rId2"/>
-    <sheet name="2025-05-21" sheetId="3" r:id="rId3"/>
-    <sheet name="2025-05-20" sheetId="2" r:id="rId4"/>
-    <sheet name="2025-05-19" sheetId="1" r:id="rId5"/>
+    <sheet name="2025-06-03" sheetId="6" r:id="rId1"/>
+    <sheet name="2025-06-02" sheetId="5" r:id="rId2"/>
+    <sheet name="2025-05-28" sheetId="4" r:id="rId3"/>
+    <sheet name="2025-05-21" sheetId="3" r:id="rId4"/>
+    <sheet name="2025-05-20" sheetId="2" r:id="rId5"/>
+    <sheet name="2025-05-19" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="2334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3348" uniqueCount="2744">
   <si>
     <t>B1</t>
   </si>
@@ -7031,6 +7032,1236 @@
   </si>
   <si>
     <t>LEC/12310/222.38</t>
+  </si>
+  <si>
+    <t>CHDC/7355/2,543.44</t>
+  </si>
+  <si>
+    <t>NIFRA/53711/285.41</t>
+  </si>
+  <si>
+    <t>EBL/21091/645.99</t>
+  </si>
+  <si>
+    <t>HPPL/23640/519.87</t>
+  </si>
+  <si>
+    <t>RNLI/21562/511.59</t>
+  </si>
+  <si>
+    <t>SHPC/28563/588.36</t>
+  </si>
+  <si>
+    <t>HIDCL/33349/306.42</t>
+  </si>
+  <si>
+    <t>SHIVM/18659/530.00</t>
+  </si>
+  <si>
+    <t>HLI/23582/413.77</t>
+  </si>
+  <si>
+    <t>SARBTM/34906/856.82</t>
+  </si>
+  <si>
+    <t>UPCL/70428/418.10</t>
+  </si>
+  <si>
+    <t>SHIVM/26266/525.95</t>
+  </si>
+  <si>
+    <t>MERO/18838/723.97</t>
+  </si>
+  <si>
+    <t>SPDL/33889/383.13</t>
+  </si>
+  <si>
+    <t>NGPL/69970/382.59</t>
+  </si>
+  <si>
+    <t>HDL/6601/1,236.45</t>
+  </si>
+  <si>
+    <t>HPPL/13727/527.87</t>
+  </si>
+  <si>
+    <t>SHPC/12251/589.15</t>
+  </si>
+  <si>
+    <t>AKPL/23797/258.47</t>
+  </si>
+  <si>
+    <t>NRIC/347219/1,293.47</t>
+  </si>
+  <si>
+    <t>HRL/57556/959.77</t>
+  </si>
+  <si>
+    <t>SAHAS/34827/525.36</t>
+  </si>
+  <si>
+    <t>SHPC/29899/588.37</t>
+  </si>
+  <si>
+    <t>NHPC/57077/226.76</t>
+  </si>
+  <si>
+    <t>CHDC/10841/2,536.06</t>
+  </si>
+  <si>
+    <t>RADHI/23979/735.98</t>
+  </si>
+  <si>
+    <t>NICA/43346/360.14</t>
+  </si>
+  <si>
+    <t>UPCL/24967/424.73</t>
+  </si>
+  <si>
+    <t>GHL/37850/259.51</t>
+  </si>
+  <si>
+    <t>LBBL/256961/453.04</t>
+  </si>
+  <si>
+    <t>BPCL/93541/552.54</t>
+  </si>
+  <si>
+    <t>SADBL/76797/429.47</t>
+  </si>
+  <si>
+    <t>LSL/98302/223.68</t>
+  </si>
+  <si>
+    <t>SINDU/16229/835.22</t>
+  </si>
+  <si>
+    <t>GHL/32573/253.27</t>
+  </si>
+  <si>
+    <t>NTC/8210/872.10</t>
+  </si>
+  <si>
+    <t>SHEL/21754/274.63</t>
+  </si>
+  <si>
+    <t>HATHY/4252/1,251.31</t>
+  </si>
+  <si>
+    <t>BARUN/26608/525.95</t>
+  </si>
+  <si>
+    <t>NGPL/34377/386.40</t>
+  </si>
+  <si>
+    <t>NABIL/26837/493.10</t>
+  </si>
+  <si>
+    <t>BHL/46838/220.68</t>
+  </si>
+  <si>
+    <t>CIT/3129/1,917.77</t>
+  </si>
+  <si>
+    <t>CREST/6266/2,002.75</t>
+  </si>
+  <si>
+    <t>SHL/19738/570.27</t>
+  </si>
+  <si>
+    <t>NMIC/5016/2,112.93</t>
+  </si>
+  <si>
+    <t>NIFRA/32651/284.32</t>
+  </si>
+  <si>
+    <t>RIDI/32352/271.74</t>
+  </si>
+  <si>
+    <t>SAHAS/62603/527.22</t>
+  </si>
+  <si>
+    <t>NGPL/55855/384.44</t>
+  </si>
+  <si>
+    <t>CREST/9358/1,950.92</t>
+  </si>
+  <si>
+    <t>NLG/20051/820.55</t>
+  </si>
+  <si>
+    <t>AHPC/50490/296.13</t>
+  </si>
+  <si>
+    <t>TPC/185183/586.04</t>
+  </si>
+  <si>
+    <t>HURJA/435086/263.31</t>
+  </si>
+  <si>
+    <t>RHPL/180291/396.03</t>
+  </si>
+  <si>
+    <t>NMIC/27415/2,045.70</t>
+  </si>
+  <si>
+    <t>CREST/18899/1,916.45</t>
+  </si>
+  <si>
+    <t>BPCL/301991/498.62</t>
+  </si>
+  <si>
+    <t>SHIVM/136140/531.19</t>
+  </si>
+  <si>
+    <t>SADBL/89397/426.00</t>
+  </si>
+  <si>
+    <t>AHPC/73131/296.52</t>
+  </si>
+  <si>
+    <t>MDB/25342/604.48</t>
+  </si>
+  <si>
+    <t>BARUN/31906/542.15</t>
+  </si>
+  <si>
+    <t>UPPER/56651/205.52</t>
+  </si>
+  <si>
+    <t>CREST/4613/2,013.27</t>
+  </si>
+  <si>
+    <t>LBBL/68174/467.00</t>
+  </si>
+  <si>
+    <t>BPCL/59071/514.40</t>
+  </si>
+  <si>
+    <t>NADEP/11120/859.66</t>
+  </si>
+  <si>
+    <t>BARUN/15778/535.85</t>
+  </si>
+  <si>
+    <t>NLG/10270/810.44</t>
+  </si>
+  <si>
+    <t>LBBL/68010/465.10</t>
+  </si>
+  <si>
+    <t>RADHI/26221/742.77</t>
+  </si>
+  <si>
+    <t>NRN/8736/2,035.89</t>
+  </si>
+  <si>
+    <t>NGPL/42199/390.98</t>
+  </si>
+  <si>
+    <t>EBL/21856/648.40</t>
+  </si>
+  <si>
+    <t>NGPL/66326/386.45</t>
+  </si>
+  <si>
+    <t>SHIVM/29888/525.21</t>
+  </si>
+  <si>
+    <t>SADBL/34965/419.69</t>
+  </si>
+  <si>
+    <t>AKJCL/63236/214.99</t>
+  </si>
+  <si>
+    <t>SAHAS/23304/520.99</t>
+  </si>
+  <si>
+    <t>SHIVM/47928/528.30</t>
+  </si>
+  <si>
+    <t>BARUN/38915/529.11</t>
+  </si>
+  <si>
+    <t>SONA/42937/461.28</t>
+  </si>
+  <si>
+    <t>HPPL/26466/531.48</t>
+  </si>
+  <si>
+    <t>KBL/204000/215.39</t>
+  </si>
+  <si>
+    <t>HIDCL/97820/305.39</t>
+  </si>
+  <si>
+    <t>SHPC/32057/604.37</t>
+  </si>
+  <si>
+    <t>NICA/31438/357.93</t>
+  </si>
+  <si>
+    <t>SHEL/32120/278.19</t>
+  </si>
+  <si>
+    <t>RADHI/71557/749.09</t>
+  </si>
+  <si>
+    <t>NRN/19206/2,080.50</t>
+  </si>
+  <si>
+    <t>BHL/106814/218.71</t>
+  </si>
+  <si>
+    <t>NGPL/59470/379.42</t>
+  </si>
+  <si>
+    <t>MEN/35492/584.09</t>
+  </si>
+  <si>
+    <t>SAHAS/162334/527.45</t>
+  </si>
+  <si>
+    <t>NGPL/121676/381.02</t>
+  </si>
+  <si>
+    <t>BPCL/70682/512.30</t>
+  </si>
+  <si>
+    <t>NABBC/15329/1,570.69</t>
+  </si>
+  <si>
+    <t>CORBL/14207/2,401.95</t>
+  </si>
+  <si>
+    <t>RADHI/108334/742.70</t>
+  </si>
+  <si>
+    <t>HURJA/70708/266.77</t>
+  </si>
+  <si>
+    <t>AHPC/62138/295.78</t>
+  </si>
+  <si>
+    <t>UMHL/33122/512.00</t>
+  </si>
+  <si>
+    <t>GRDBL/13013/1,258.63</t>
+  </si>
+  <si>
+    <t>UPCL/338173/430.42</t>
+  </si>
+  <si>
+    <t>CHDC/57225/2,564.83</t>
+  </si>
+  <si>
+    <t>HIDCL/130375/305.29</t>
+  </si>
+  <si>
+    <t>SHL/31792/579.91</t>
+  </si>
+  <si>
+    <t>NGPL/33112/384.68</t>
+  </si>
+  <si>
+    <t>SBL/500340/292.53</t>
+  </si>
+  <si>
+    <t>EBL/126801/652.86</t>
+  </si>
+  <si>
+    <t>RADHI/109975/749.89</t>
+  </si>
+  <si>
+    <t>HRL/55308/970.70</t>
+  </si>
+  <si>
+    <t>API/316073/303.78</t>
+  </si>
+  <si>
+    <t>HIDCL/137659/307.70</t>
+  </si>
+  <si>
+    <t>MEN/60285/588.10</t>
+  </si>
+  <si>
+    <t>ALICL/43381/714.02</t>
+  </si>
+  <si>
+    <t>NIFRA/102831/283.86</t>
+  </si>
+  <si>
+    <t>GBIME/244859/239.41</t>
+  </si>
+  <si>
+    <t>UPCL/68441/418.88</t>
+  </si>
+  <si>
+    <t>NIFRA/93180/281.61</t>
+  </si>
+  <si>
+    <t>HDHPC/103004/213.88</t>
+  </si>
+  <si>
+    <t>RADHI/26123/746.85</t>
+  </si>
+  <si>
+    <t>SBI/137926/406.89</t>
+  </si>
+  <si>
+    <t>EBL/37805/625.30</t>
+  </si>
+  <si>
+    <t>SHEL/61024/279.85</t>
+  </si>
+  <si>
+    <t>JBBL/42227/336.39</t>
+  </si>
+  <si>
+    <t>KBL/57552/211.74</t>
+  </si>
+  <si>
+    <t>MEN/11794/584.31</t>
+  </si>
+  <si>
+    <t>SHPC/8692/591.38</t>
+  </si>
+  <si>
+    <t>BHPL/4655/953.55</t>
+  </si>
+  <si>
+    <t>SAHAS/8421/522.61</t>
+  </si>
+  <si>
+    <t>RIDI/12026/270.82</t>
+  </si>
+  <si>
+    <t>BPCL/218837/521.75</t>
+  </si>
+  <si>
+    <t>SHIVM/74002/527.28</t>
+  </si>
+  <si>
+    <t>CHDC/12417/2,538.11</t>
+  </si>
+  <si>
+    <t>ULBSL/6371/3,346.88</t>
+  </si>
+  <si>
+    <t>HPPL/40992/518.75</t>
+  </si>
+  <si>
+    <t>RADHI/258220/717.22</t>
+  </si>
+  <si>
+    <t>NRN/67535/2,064.96</t>
+  </si>
+  <si>
+    <t>UPCL/236830/422.82</t>
+  </si>
+  <si>
+    <t>BARUN/27747/529.02</t>
+  </si>
+  <si>
+    <t>SPDL/35337/387.48</t>
+  </si>
+  <si>
+    <t>BPCL/133828/501.63</t>
+  </si>
+  <si>
+    <t>SANIMA/47494/316.20</t>
+  </si>
+  <si>
+    <t>MEN/23430/592.78</t>
+  </si>
+  <si>
+    <t>CHDC/4145/2,542.17</t>
+  </si>
+  <si>
+    <t>SHPC/16109/584.44</t>
+  </si>
+  <si>
+    <t>SAPDBL/82184/942.73</t>
+  </si>
+  <si>
+    <t>GRDBL/26460/1,217.71</t>
+  </si>
+  <si>
+    <t>SINDU/32833/886.72</t>
+  </si>
+  <si>
+    <t>NMIC/13918/2,090.36</t>
+  </si>
+  <si>
+    <t>SHIVM/46581/528.15</t>
+  </si>
+  <si>
+    <t>GBIME/784388/239.20</t>
+  </si>
+  <si>
+    <t>AKPL/369481/255.95</t>
+  </si>
+  <si>
+    <t>RADHI/99995/757.00</t>
+  </si>
+  <si>
+    <t>MERO/107325/743.97</t>
+  </si>
+  <si>
+    <t>SHPC/112257/597.38</t>
+  </si>
+  <si>
+    <t>BPCL/106336/516.38</t>
+  </si>
+  <si>
+    <t>SPIL/29206/822.37</t>
+  </si>
+  <si>
+    <t>USLB/11379/1,949.34</t>
+  </si>
+  <si>
+    <t>SHIVM/32850/532.08</t>
+  </si>
+  <si>
+    <t>MEN/27291/590.32</t>
+  </si>
+  <si>
+    <t>EBL/145521/651.63</t>
+  </si>
+  <si>
+    <t>HRL/62325/968.62</t>
+  </si>
+  <si>
+    <t>PPCL/142064/342.90</t>
+  </si>
+  <si>
+    <t>MLBL/115694/394.56</t>
+  </si>
+  <si>
+    <t>SHPC/81275/588.07</t>
+  </si>
+  <si>
+    <t>SHPC/798331/594.91</t>
+  </si>
+  <si>
+    <t>NLIC/58807/758.78</t>
+  </si>
+  <si>
+    <t>CZBIL/198917/215.74</t>
+  </si>
+  <si>
+    <t>GBIME/169188/224.81</t>
+  </si>
+  <si>
+    <t>CHDC/12252/2,575.96</t>
+  </si>
+  <si>
+    <t>API/52438/303.58</t>
+  </si>
+  <si>
+    <t>HIDCL/30736/296.37</t>
+  </si>
+  <si>
+    <t>AKPL/23142/251.51</t>
+  </si>
+  <si>
+    <t>AHPC/145707/296.15</t>
+  </si>
+  <si>
+    <t>SPDL/35771/385.23</t>
+  </si>
+  <si>
+    <t>CREST/6531/1,980.20</t>
+  </si>
+  <si>
+    <t>HRL/12158/961.29</t>
+  </si>
+  <si>
+    <t>SHL/20183/565.87</t>
+  </si>
+  <si>
+    <t>SHL/212759/569.41</t>
+  </si>
+  <si>
+    <t>SHPC/86565/589.75</t>
+  </si>
+  <si>
+    <t>AHPC/88748/299.13</t>
+  </si>
+  <si>
+    <t>SHIVM/45364/527.56</t>
+  </si>
+  <si>
+    <t>NGPL/45286/384.02</t>
+  </si>
+  <si>
+    <t>RADHI/64759/731.74</t>
+  </si>
+  <si>
+    <t>SHPC/74538/595.67</t>
+  </si>
+  <si>
+    <t>MEN/75573/583.35</t>
+  </si>
+  <si>
+    <t>HPPL/45248/531.06</t>
+  </si>
+  <si>
+    <t>NTC/27886/870.10</t>
+  </si>
+  <si>
+    <t>RADHI/386501/745.33</t>
+  </si>
+  <si>
+    <t>SHL/55565/577.48</t>
+  </si>
+  <si>
+    <t>SHEL/89561/284.15</t>
+  </si>
+  <si>
+    <t>HURJA/70813/261.15</t>
+  </si>
+  <si>
+    <t>SPIL/22927/804.88</t>
+  </si>
+  <si>
+    <t>CHDC/19537/2,583.83</t>
+  </si>
+  <si>
+    <t>AHPC/74973/295.63</t>
+  </si>
+  <si>
+    <t>AKPL/78334/251.82</t>
+  </si>
+  <si>
+    <t>API/34983/305.60</t>
+  </si>
+  <si>
+    <t>BHL/35820/219.13</t>
+  </si>
+  <si>
+    <t>CHDC/12463/2,584.20</t>
+  </si>
+  <si>
+    <t>API/27685/307.48</t>
+  </si>
+  <si>
+    <t>RNLI/16911/509.65</t>
+  </si>
+  <si>
+    <t>BHL/37361/218.46</t>
+  </si>
+  <si>
+    <t>NIFRA/25854/284.76</t>
+  </si>
+  <si>
+    <t>NMIC/5335/2,083.39</t>
+  </si>
+  <si>
+    <t>MEN/17576/597.71</t>
+  </si>
+  <si>
+    <t>UMHL/17157/513.76</t>
+  </si>
+  <si>
+    <t>ULBSL/2648/3,329.00</t>
+  </si>
+  <si>
+    <t>SHPC/12179/599.13</t>
+  </si>
+  <si>
+    <t>STC/12629/5,082.01</t>
+  </si>
+  <si>
+    <t>SADBL/30389/422.60</t>
+  </si>
+  <si>
+    <t>BARUN/19804/537.27</t>
+  </si>
+  <si>
+    <t>CBBL/12681/856.93</t>
+  </si>
+  <si>
+    <t>BHL/35243/219.48</t>
+  </si>
+  <si>
+    <t>GMLI/178280/2,593.04</t>
+  </si>
+  <si>
+    <t>NRIC/248146/1,293.13</t>
+  </si>
+  <si>
+    <t>NMIC/46938/1,963.22</t>
+  </si>
+  <si>
+    <t>HDL/17329/1,218.98</t>
+  </si>
+  <si>
+    <t>RADHI/86357/762.77</t>
+  </si>
+  <si>
+    <t>NGPL/85927/387.65</t>
+  </si>
+  <si>
+    <t>SMHL/34061/944.29</t>
+  </si>
+  <si>
+    <t>BEDC/41113/720.52</t>
+  </si>
+  <si>
+    <t>MKCL/15423/1,543.55</t>
+  </si>
+  <si>
+    <t>NGPL/187777/383.35</t>
+  </si>
+  <si>
+    <t>RADHI/31842/740.38</t>
+  </si>
+  <si>
+    <t>AHPC/65864/295.37</t>
+  </si>
+  <si>
+    <t>HDHPC/97627/205.49</t>
+  </si>
+  <si>
+    <t>GHL/78427/254.65</t>
+  </si>
+  <si>
+    <t>KBL/1685747/214.45</t>
+  </si>
+  <si>
+    <t>NRN/142686/2,045.00</t>
+  </si>
+  <si>
+    <t>AHPC/408602/298.59</t>
+  </si>
+  <si>
+    <t>NGPL/320939/383.45</t>
+  </si>
+  <si>
+    <t>OHL/109000/949.54</t>
+  </si>
+  <si>
+    <t>SHPC/37057/596.06</t>
+  </si>
+  <si>
+    <t>NGPL/54793/383.58</t>
+  </si>
+  <si>
+    <t>NIFRA/58285/286.31</t>
+  </si>
+  <si>
+    <t>API/51760/304.03</t>
+  </si>
+  <si>
+    <t>RADHI/105468/747.27</t>
+  </si>
+  <si>
+    <t>UPCL/145987/423.92</t>
+  </si>
+  <si>
+    <t>SHL/62049/569.11</t>
+  </si>
+  <si>
+    <t>LBBL/50062/474.52</t>
+  </si>
+  <si>
+    <t>SHPC/36778/584.13</t>
+  </si>
+  <si>
+    <t>SHL/23318/567.63</t>
+  </si>
+  <si>
+    <t>CREST/4430/1,948.84</t>
+  </si>
+  <si>
+    <t>NMIC/4146/2,032.52</t>
+  </si>
+  <si>
+    <t>SADBL/11828/423.13</t>
+  </si>
+  <si>
+    <t>UMHL/444936/505.23</t>
+  </si>
+  <si>
+    <t>RIDI/277526/269.63</t>
+  </si>
+  <si>
+    <t>BPCL/66774/532.22</t>
+  </si>
+  <si>
+    <t>MKHL/33677/711.29</t>
+  </si>
+  <si>
+    <t>SHIVM/43070/533.21</t>
+  </si>
+  <si>
+    <t>RADHI/27527/747.58</t>
+  </si>
+  <si>
+    <t>SHEL/48245/285.38</t>
+  </si>
+  <si>
+    <t>SHL/22837/562.51</t>
+  </si>
+  <si>
+    <t>KBL/47999/211.69</t>
+  </si>
+  <si>
+    <t>PPCL/28946/344.60</t>
+  </si>
+  <si>
+    <t>BPCL/223390/520.11</t>
+  </si>
+  <si>
+    <t>SHPC/107064/599.73</t>
+  </si>
+  <si>
+    <t>BEDC/60051/741.85</t>
+  </si>
+  <si>
+    <t>NRN/18147/2,064.26</t>
+  </si>
+  <si>
+    <t>LSL/163025/214.45</t>
+  </si>
+  <si>
+    <t>PHCL/56590/600.37</t>
+  </si>
+  <si>
+    <t>SANIMA/101200/318.89</t>
+  </si>
+  <si>
+    <t>NGPL/77881/385.29</t>
+  </si>
+  <si>
+    <t>CHDC/44944/2,576.46</t>
+  </si>
+  <si>
+    <t>NRN/22016/2,065.78</t>
+  </si>
+  <si>
+    <t>NGPL/75399/375.89</t>
+  </si>
+  <si>
+    <t>UHEWA/35840/628.89</t>
+  </si>
+  <si>
+    <t>HIDCL/65055/297.05</t>
+  </si>
+  <si>
+    <t>RADHI/113328/764.25</t>
+  </si>
+  <si>
+    <t>HIDCL/83248/303.59</t>
+  </si>
+  <si>
+    <t>SHIVM/25485/535.81</t>
+  </si>
+  <si>
+    <t>HRL/8994/962.33</t>
+  </si>
+  <si>
+    <t>SHEL/22663/283.20</t>
+  </si>
+  <si>
+    <t>NGPL/127911/382.95</t>
+  </si>
+  <si>
+    <t>AHPC/71002/291.82</t>
+  </si>
+  <si>
+    <t>RIDI/66112/263.06</t>
+  </si>
+  <si>
+    <t>HIDCL/50241/305.46</t>
+  </si>
+  <si>
+    <t>SHPC/17108/597.20</t>
+  </si>
+  <si>
+    <t>HIDCL/74686/306.79</t>
+  </si>
+  <si>
+    <t>BPCL/77945/561.06</t>
+  </si>
+  <si>
+    <t>SHPC/43198/590.62</t>
+  </si>
+  <si>
+    <t>RADHI/15561/751.90</t>
+  </si>
+  <si>
+    <t>RADHI/94012/737.54</t>
+  </si>
+  <si>
+    <t>UPCL/117034/425.37</t>
+  </si>
+  <si>
+    <t>LBBL/97601/465.64</t>
+  </si>
+  <si>
+    <t>API/99611/306.39</t>
+  </si>
+  <si>
+    <t>SAPDBL/16577/908.26</t>
+  </si>
+  <si>
+    <t>CORBL/55666/2,278.00</t>
+  </si>
+  <si>
+    <t>GRDBL/27721/1,156.50</t>
+  </si>
+  <si>
+    <t>NRN/10576/2,064.29</t>
+  </si>
+  <si>
+    <t>CHDC/8504/2,565.04</t>
+  </si>
+  <si>
+    <t>TVCL/700/472.71</t>
+  </si>
+  <si>
+    <t>SONA/351/455.47</t>
+  </si>
+  <si>
+    <t>HURJA/500/247.80</t>
+  </si>
+  <si>
+    <t>SHPC/77351/581.82</t>
+  </si>
+  <si>
+    <t>UPCL/51721/417.57</t>
+  </si>
+  <si>
+    <t>BNHC/24551/518.72</t>
+  </si>
+  <si>
+    <t>SKBBL/14818/803.81</t>
+  </si>
+  <si>
+    <t>NRN/19818/2,078.41</t>
+  </si>
+  <si>
+    <t>API/57332/304.95</t>
+  </si>
+  <si>
+    <t>NGPL/30735/382.54</t>
+  </si>
+  <si>
+    <t>BPCL/20600/546.82</t>
+  </si>
+  <si>
+    <t>RADHI/28723/730.19</t>
+  </si>
+  <si>
+    <t>MBJC/27025/317.22</t>
+  </si>
+  <si>
+    <t>SHIVM/11771/526.10</t>
+  </si>
+  <si>
+    <t>MEN/7636/577.27</t>
+  </si>
+  <si>
+    <t>CHDC/36991/2,567.21</t>
+  </si>
+  <si>
+    <t>BPCL/135506/524.30</t>
+  </si>
+  <si>
+    <t>NRN/28481/2,061.44</t>
+  </si>
+  <si>
+    <t>RADHI/73180/755.21</t>
+  </si>
+  <si>
+    <t>LBBL/70074/470.58</t>
+  </si>
+  <si>
+    <t>RADHI/7472/757.05</t>
+  </si>
+  <si>
+    <t>ALICL/7384/708.65</t>
+  </si>
+  <si>
+    <t>NGPL/8245/379.91</t>
+  </si>
+  <si>
+    <t>MEN/50894/585.11</t>
+  </si>
+  <si>
+    <t>NIFRA/84303/287.58</t>
+  </si>
+  <si>
+    <t>NMLBBL/30141/664.33</t>
+  </si>
+  <si>
+    <t>RADHI/17869/756.43</t>
+  </si>
+  <si>
+    <t>HRL/12002/974.21</t>
+  </si>
+  <si>
+    <t>UPCL/243889/422.70</t>
+  </si>
+  <si>
+    <t>NGPL/219706/390.87</t>
+  </si>
+  <si>
+    <t>RIDI/134406/270.96</t>
+  </si>
+  <si>
+    <t>HRL/16921/983.17</t>
+  </si>
+  <si>
+    <t>NRN/15709/2,063.17</t>
+  </si>
+  <si>
+    <t>NICA/42799/372.17</t>
+  </si>
+  <si>
+    <t>UMHL/16692/509.84</t>
+  </si>
+  <si>
+    <t>BPCL/13201/541.81</t>
+  </si>
+  <si>
+    <t>RADHI/10399/743.93</t>
+  </si>
+  <si>
+    <t>RADHI/27956/750.73</t>
+  </si>
+  <si>
+    <t>HRL/15480/960.40</t>
+  </si>
+  <si>
+    <t>KPCL/15914/523.81</t>
+  </si>
+  <si>
+    <t>HIDCL/96075/302.17</t>
+  </si>
+  <si>
+    <t>SADBL/48621/422.43</t>
+  </si>
+  <si>
+    <t>KSBBL/39511/446.86</t>
+  </si>
+  <si>
+    <t>HDL/12425/1,217.87</t>
+  </si>
+  <si>
+    <t>NGPL/175415/380.91</t>
+  </si>
+  <si>
+    <t>SHL/71323/585.22</t>
+  </si>
+  <si>
+    <t>RADHI/53957/751.06</t>
+  </si>
+  <si>
+    <t>NRN/6761/2,078.97</t>
+  </si>
+  <si>
+    <t>SHEL/42683/282.85</t>
+  </si>
+  <si>
+    <t>UPCL/36702/414.81</t>
+  </si>
+  <si>
+    <t>NGPL/35347/385.21</t>
+  </si>
+  <si>
+    <t>NRIC/9167/1,284.54</t>
+  </si>
+  <si>
+    <t>RADHI/15436/750.97</t>
+  </si>
+  <si>
+    <t>RADHI/90846/746.47</t>
+  </si>
+  <si>
+    <t>NMIC/4316/2,070.67</t>
+  </si>
+  <si>
+    <t>UPCL/13062/416.58</t>
+  </si>
+  <si>
+    <t>HURJA/10465/273.32</t>
+  </si>
+  <si>
+    <t>SAPDBL/31931/905.26</t>
+  </si>
+  <si>
+    <t>SHPC/25673/587.63</t>
+  </si>
+  <si>
+    <t>CORBL/5200/2,579.05</t>
+  </si>
+  <si>
+    <t>GRDBL/10132/1,176.96</t>
+  </si>
+  <si>
+    <t>BARUN/13620/536.07</t>
+  </si>
+  <si>
+    <t>RADHI/35681/739.58</t>
+  </si>
+  <si>
+    <t>GBIME/87094/236.22</t>
+  </si>
+  <si>
+    <t>NGPL/22205/380.66</t>
+  </si>
+  <si>
+    <t>HRL/2792/975.04</t>
+  </si>
+  <si>
+    <t>SHL/10859/573.68</t>
+  </si>
+  <si>
+    <t>BARUN/5280/540.34</t>
+  </si>
+  <si>
+    <t>CREST/1330/1,908.34</t>
+  </si>
+  <si>
+    <t>AHPC/7826/293.93</t>
+  </si>
+  <si>
+    <t>UPCL/61953/424.75</t>
+  </si>
+  <si>
+    <t>RADHI/19349/745.59</t>
+  </si>
+  <si>
+    <t>BPCL/25662/526.43</t>
+  </si>
+  <si>
+    <t>SHPC/19692/585.15</t>
+  </si>
+  <si>
+    <t>AKPL/43010/257.07</t>
+  </si>
+  <si>
+    <t>HIDCL/159221/300.55</t>
+  </si>
+  <si>
+    <t>RADHI/7185/741.66</t>
+  </si>
+  <si>
+    <t>SPHL/5991/696.42</t>
+  </si>
+  <si>
+    <t>HEI/13324/582.80</t>
+  </si>
+  <si>
+    <t>ICFC/6430/616.12</t>
+  </si>
+  <si>
+    <t>HRL/3713/972.03</t>
+  </si>
+  <si>
+    <t>SHPC/5910/592.48</t>
+  </si>
+  <si>
+    <t>BPCL/10240/475.77</t>
+  </si>
+  <si>
+    <t>RADHI/192871/757.12</t>
+  </si>
+  <si>
+    <t>MKHL/126331/723.02</t>
+  </si>
+  <si>
+    <t>UPCL/76690/420.70</t>
+  </si>
+  <si>
+    <t>NGPL/87845/379.12</t>
+  </si>
+  <si>
+    <t>PRIN/33202/868.25</t>
+  </si>
+  <si>
+    <t>UPCL/56807/437.46</t>
+  </si>
+  <si>
+    <t>NMIC/3590/2,173.38</t>
+  </si>
+  <si>
+    <t>NICA/17864/366.34</t>
+  </si>
+  <si>
+    <t>NMB/25956/240.58</t>
+  </si>
+  <si>
+    <t>NLG/7565/777.64</t>
+  </si>
+  <si>
+    <t>LBBL/175446/469.87</t>
+  </si>
+  <si>
+    <t>SHL/88564/561.64</t>
+  </si>
+  <si>
+    <t>NICA/108981/366.30</t>
+  </si>
+  <si>
+    <t>NRN/8628/2,051.00</t>
+  </si>
+  <si>
+    <t>SHPC/27257/591.02</t>
+  </si>
+  <si>
+    <t>UPCL/24749/432.15</t>
+  </si>
+  <si>
+    <t>SADBL/21210/431.15</t>
+  </si>
+  <si>
+    <t>NMIC/3468/2,101.53</t>
+  </si>
+  <si>
+    <t>NGPL/51323/384.12</t>
+  </si>
+  <si>
+    <t>API/49730/309.58</t>
+  </si>
+  <si>
+    <t>SHPC/21973/577.85</t>
+  </si>
+  <si>
+    <t>AHPC/26010/292.41</t>
+  </si>
+  <si>
+    <t>SHIVM/24148/536.43</t>
+  </si>
+  <si>
+    <t>BPCL/18885/556.62</t>
+  </si>
+  <si>
+    <t>UPCL/17961/420.40</t>
+  </si>
+  <si>
+    <t>PHCL/109404/605.37</t>
+  </si>
+  <si>
+    <t>MLBL/46873/389.48</t>
+  </si>
+  <si>
+    <t>RADHI/18362/781.26</t>
+  </si>
+  <si>
+    <t>CHDC/4147/2,576.84</t>
+  </si>
+  <si>
+    <t>NGPL/15702/390.27</t>
+  </si>
+  <si>
+    <t>RADHI/7567/731.57</t>
+  </si>
+  <si>
+    <t>RFPL/7536/479.68</t>
   </si>
 </sst>
 </file>
@@ -7353,11 +8584,1893 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676205A0-C5FF-4AEC-B10B-18D60F60A28C}">
+  <dimension ref="A1:F93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2335</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2336</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2339</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2340</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2341</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2342</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2343</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2346</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2348</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2349</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2350</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2351</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2353</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2355</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2358</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2360</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2361</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2365</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2366</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2368</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2370</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1923</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2372</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2373</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2374</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2375</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2378</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2379</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2380</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2382</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2384</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2385</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2387</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2389</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2390</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2392</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2393</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2394</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2395</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2398</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2400</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2401</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2402</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2403</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2407</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2408</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2411</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2412</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2413</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2417</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2418</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2420</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2421</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2422</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2426</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2427</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2430</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2431</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2432</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2436</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2437</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2442</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2444</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2445</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2446</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2447</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2450</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2451</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2454</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2455</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2456</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2458</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2460</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2461</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2464</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2465</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2466</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2470</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2471</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2473</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2474</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2475</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2476</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2479</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2480</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2481</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2485</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2486</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2491</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2494</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2496</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2501</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2505</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2506</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2508</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2509</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2069</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2070</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2513</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2514</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2516</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2518</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2519</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2522</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2524</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2527</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2528</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2529</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2532</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2533</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2534</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2537</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2538</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2539</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2543</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2544</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2548</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2549</v>
+      </c>
+      <c r="F46" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2552</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2114</v>
+      </c>
+      <c r="F47" t="s">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2555</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2556</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2557</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2558</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2562</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2563</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>288</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2566</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2567</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2568</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2571</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2572</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>300</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2576</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2577</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>306</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>312</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2584</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2585</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2586</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2588</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2589</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2590</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2591</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2594</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2595</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2596</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>330</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2599</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>336</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2603</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2604</v>
+      </c>
+      <c r="F58" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>342</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2606</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2607</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2609</v>
+      </c>
+      <c r="F59" t="s">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>348</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2611</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2613</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2614</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>354</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2181</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2182</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2616</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2184</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>360</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2617</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2618</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2188</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2619</v>
+      </c>
+      <c r="F62" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>366</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2620</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2622</v>
+      </c>
+      <c r="E63" t="s">
+        <v>2623</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>372</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2625</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2197</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2626</v>
+      </c>
+      <c r="E64" t="s">
+        <v>2627</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2628</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>378</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2629</v>
+      </c>
+      <c r="C65" t="s">
+        <v>381</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2630</v>
+      </c>
+      <c r="E65" t="s">
+        <v>2631</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2632</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2634</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F66" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>390</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2636</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2637</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2210</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2638</v>
+      </c>
+      <c r="F67" t="s">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>396</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2641</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2642</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F68" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2644</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2645</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2646</v>
+      </c>
+      <c r="E69" t="s">
+        <v>2647</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>408</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2649</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E70" t="s">
+        <v>2651</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>414</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1776</v>
+      </c>
+      <c r="E71" t="s">
+        <v>2226</v>
+      </c>
+      <c r="F71" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>420</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2653</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2654</v>
+      </c>
+      <c r="E72" t="s">
+        <v>2655</v>
+      </c>
+      <c r="F72" t="s">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>426</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D73" t="s">
+        <v>2234</v>
+      </c>
+      <c r="E73" t="s">
+        <v>2659</v>
+      </c>
+      <c r="F73" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>432</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2663</v>
+      </c>
+      <c r="E74" t="s">
+        <v>2664</v>
+      </c>
+      <c r="F74" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>438</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2666</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2667</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2668</v>
+      </c>
+      <c r="E75" t="s">
+        <v>2244</v>
+      </c>
+      <c r="F75" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>444</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2669</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2670</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2671</v>
+      </c>
+      <c r="E76" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F76" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>450</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D77" t="s">
+        <v>2675</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2676</v>
+      </c>
+      <c r="F77" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>456</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2678</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2679</v>
+      </c>
+      <c r="E78" t="s">
+        <v>2680</v>
+      </c>
+      <c r="F78" t="s">
+        <v>2681</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>462</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2682</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2683</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2264</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2684</v>
+      </c>
+      <c r="F79" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>468</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2686</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2687</v>
+      </c>
+      <c r="D80" t="s">
+        <v>2688</v>
+      </c>
+      <c r="E80" t="s">
+        <v>2689</v>
+      </c>
+      <c r="F80" t="s">
+        <v>2690</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>474</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2691</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2692</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2693</v>
+      </c>
+      <c r="E81" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F81" t="s">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>480</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2696</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2697</v>
+      </c>
+      <c r="F82" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>486</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2699</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2700</v>
+      </c>
+      <c r="D83" t="s">
+        <v>2701</v>
+      </c>
+      <c r="E83" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F83" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>492</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2704</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D84" t="s">
+        <v>2289</v>
+      </c>
+      <c r="E84" t="s">
+        <v>2705</v>
+      </c>
+      <c r="F84" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>498</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2707</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D85" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E85" t="s">
+        <v>2710</v>
+      </c>
+      <c r="F85" t="s">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>504</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2712</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2713</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2714</v>
+      </c>
+      <c r="E86" t="s">
+        <v>2715</v>
+      </c>
+      <c r="F86" t="s">
+        <v>2716</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>510</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2717</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2718</v>
+      </c>
+      <c r="D87" t="s">
+        <v>2719</v>
+      </c>
+      <c r="E87" t="s">
+        <v>2720</v>
+      </c>
+      <c r="F87" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>516</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2723</v>
+      </c>
+      <c r="D88" t="s">
+        <v>2724</v>
+      </c>
+      <c r="E88" t="s">
+        <v>2308</v>
+      </c>
+      <c r="F88" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>522</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2725</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2726</v>
+      </c>
+      <c r="D89" t="s">
+        <v>2727</v>
+      </c>
+      <c r="E89" t="s">
+        <v>2728</v>
+      </c>
+      <c r="F89" t="s">
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>528</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D90" t="s">
+        <v>2731</v>
+      </c>
+      <c r="E90" t="s">
+        <v>2732</v>
+      </c>
+      <c r="F90" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>534</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2734</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D91" t="s">
+        <v>2735</v>
+      </c>
+      <c r="E91" t="s">
+        <v>2736</v>
+      </c>
+      <c r="F91" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>540</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2737</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2738</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2739</v>
+      </c>
+      <c r="E92" t="s">
+        <v>2328</v>
+      </c>
+      <c r="F92" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>546</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2740</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2741</v>
+      </c>
+      <c r="D93" t="s">
+        <v>2742</v>
+      </c>
+      <c r="E93" t="s">
+        <v>2743</v>
+      </c>
+      <c r="F93" t="s">
+        <v>2332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FC7E8D-1DE3-4DBF-BC92-6657EED87D10}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9235,7 +12348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEF453-2C93-48DA-92A9-F02917F02C21}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -11117,7 +14230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3009EEF-D0A3-4418-BB02-D308992E6389}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -12997,7 +16110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62503B16-5D5E-43EB-8EDC-28C65E9BFBAD}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -14877,7 +17990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F93"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Broker Analysis.xlsx 	modified:   Broker holdings.py
</commit_message>
<xml_diff>
--- a/Broker Analysis.xlsx
+++ b/Broker Analysis.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\OneDrive\Desktop\Others\python scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FCF239-A4DB-4C66-9BC4-F17A54CD5FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AF57EF-A488-4A33-AE43-5CECB340099F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2025-06-04" sheetId="7" r:id="rId1"/>
-    <sheet name="2025-06-03" sheetId="6" r:id="rId2"/>
-    <sheet name="2025-06-02" sheetId="5" r:id="rId3"/>
-    <sheet name="2025-05-28" sheetId="4" r:id="rId4"/>
-    <sheet name="2025-05-21" sheetId="3" r:id="rId5"/>
-    <sheet name="2025-05-20" sheetId="2" r:id="rId6"/>
-    <sheet name="2025-05-19" sheetId="1" r:id="rId7"/>
+    <sheet name="2025-06-05" sheetId="8" r:id="rId1"/>
+    <sheet name="2025-06-04" sheetId="7" r:id="rId2"/>
+    <sheet name="2025-06-03" sheetId="6" r:id="rId3"/>
+    <sheet name="2025-06-02" sheetId="5" r:id="rId4"/>
+    <sheet name="2025-05-28" sheetId="4" r:id="rId5"/>
+    <sheet name="2025-05-21" sheetId="3" r:id="rId6"/>
+    <sheet name="2025-05-20" sheetId="2" r:id="rId7"/>
+    <sheet name="2025-05-19" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3906" uniqueCount="3140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4464" uniqueCount="3579">
   <si>
     <t>B1</t>
   </si>
@@ -9451,6 +9452,1323 @@
   </si>
   <si>
     <t>RFPL/12536/475.82</t>
+  </si>
+  <si>
+    <t>CHDC/7995/2,542.41</t>
+  </si>
+  <si>
+    <t>NIFRA/49080/285.15</t>
+  </si>
+  <si>
+    <t>HPPL/25730/518.68</t>
+  </si>
+  <si>
+    <t>EBL/19619/647.58</t>
+  </si>
+  <si>
+    <t>SHIVM/21393/525.56</t>
+  </si>
+  <si>
+    <t>SHPC/26393/588.19</t>
+  </si>
+  <si>
+    <t>HPPL/21851/522.45</t>
+  </si>
+  <si>
+    <t>SHIVM/19256/529.62</t>
+  </si>
+  <si>
+    <t>HLI/23682/413.73</t>
+  </si>
+  <si>
+    <t>SARBTM/5873/863.26</t>
+  </si>
+  <si>
+    <t>SARBTM/49266/853.38</t>
+  </si>
+  <si>
+    <t>UPCL/52043/419.00</t>
+  </si>
+  <si>
+    <t>MERO/18610/723.97</t>
+  </si>
+  <si>
+    <t>SHIVM/25767/525.59</t>
+  </si>
+  <si>
+    <t>SPDL/31860/381.04</t>
+  </si>
+  <si>
+    <t>NGPL/55224/383.30</t>
+  </si>
+  <si>
+    <t>HDL/7218/1,234.52</t>
+  </si>
+  <si>
+    <t>SHPC/11423/588.71</t>
+  </si>
+  <si>
+    <t>CREST/3401/1,944.73</t>
+  </si>
+  <si>
+    <t>HPPL/11809/522.54</t>
+  </si>
+  <si>
+    <t>NRIC/352927/1,292.77</t>
+  </si>
+  <si>
+    <t>HRL/63637/956.27</t>
+  </si>
+  <si>
+    <t>SAHAS/41687/525.33</t>
+  </si>
+  <si>
+    <t>MEN/24443/585.14</t>
+  </si>
+  <si>
+    <t>NHPC/42809/225.45</t>
+  </si>
+  <si>
+    <t>CHDC/11194/2,534.08</t>
+  </si>
+  <si>
+    <t>RADHI/27072/739.07</t>
+  </si>
+  <si>
+    <t>NICA/43928/360.13</t>
+  </si>
+  <si>
+    <t>UPCL/26229/428.62</t>
+  </si>
+  <si>
+    <t>SHPC/21171/595.61</t>
+  </si>
+  <si>
+    <t>LBBL/256958/453.01</t>
+  </si>
+  <si>
+    <t>BPCL/79755/558.60</t>
+  </si>
+  <si>
+    <t>SADBL/78445/427.11</t>
+  </si>
+  <si>
+    <t>LSL/98697/223.65</t>
+  </si>
+  <si>
+    <t>BARUN/34205/489.12</t>
+  </si>
+  <si>
+    <t>CIT/3438/1,923.71</t>
+  </si>
+  <si>
+    <t>GHL/25573/251.97</t>
+  </si>
+  <si>
+    <t>NLICL/7772/623.89</t>
+  </si>
+  <si>
+    <t>HATHY/3828/1,247.57</t>
+  </si>
+  <si>
+    <t>NABIL/27103/493.51</t>
+  </si>
+  <si>
+    <t>NGPL/32421/386.66</t>
+  </si>
+  <si>
+    <t>BARUN/18422/509.54</t>
+  </si>
+  <si>
+    <t>BHL/41007/220.00</t>
+  </si>
+  <si>
+    <t>CIT/3047/1,917.31</t>
+  </si>
+  <si>
+    <t>CREST/6931/1,996.17</t>
+  </si>
+  <si>
+    <t>HRL/11704/975.68</t>
+  </si>
+  <si>
+    <t>NMIC/5455/2,098.25</t>
+  </si>
+  <si>
+    <t>SHL/17284/571.54</t>
+  </si>
+  <si>
+    <t>RIDI/33544/271.51</t>
+  </si>
+  <si>
+    <t>SAHAS/71784/527.41</t>
+  </si>
+  <si>
+    <t>AHPC/76534/591.63</t>
+  </si>
+  <si>
+    <t>NGPL/46258/385.09</t>
+  </si>
+  <si>
+    <t>NLG/21707/815.42</t>
+  </si>
+  <si>
+    <t>CREST/8338/1,932.43</t>
+  </si>
+  <si>
+    <t>TPC/176807/586.67</t>
+  </si>
+  <si>
+    <t>HURJA/346719/262.37</t>
+  </si>
+  <si>
+    <t>RHPL/174372/396.00</t>
+  </si>
+  <si>
+    <t>NMIC/30767/2,023.02</t>
+  </si>
+  <si>
+    <t>CREST/18802/1,915.83</t>
+  </si>
+  <si>
+    <t>BPCL/285087/510.13</t>
+  </si>
+  <si>
+    <t>SHIVM/132226/531.22</t>
+  </si>
+  <si>
+    <t>AHPC/146602/591.48</t>
+  </si>
+  <si>
+    <t>SADBL/95690/425.32</t>
+  </si>
+  <si>
+    <t>BARUN/41493/488.13</t>
+  </si>
+  <si>
+    <t>UPPER/59081/205.39</t>
+  </si>
+  <si>
+    <t>CREST/4549/2,001.51</t>
+  </si>
+  <si>
+    <t>NLICL/12083/631.91</t>
+  </si>
+  <si>
+    <t>SPDL/19795/376.28</t>
+  </si>
+  <si>
+    <t>BPCL/97011/537.95</t>
+  </si>
+  <si>
+    <t>LBBL/48297/467.00</t>
+  </si>
+  <si>
+    <t>OMPL/8310/1,831.07</t>
+  </si>
+  <si>
+    <t>AKJCL/49912/426.78</t>
+  </si>
+  <si>
+    <t>SHIVM/18445/529.43</t>
+  </si>
+  <si>
+    <t>RADHI/25861/745.29</t>
+  </si>
+  <si>
+    <t>UMHL/30274/502.07</t>
+  </si>
+  <si>
+    <t>SARBTM/16700/851.51</t>
+  </si>
+  <si>
+    <t>NGPL/80339/386.94</t>
+  </si>
+  <si>
+    <t>AKJCL/121712/429.61</t>
+  </si>
+  <si>
+    <t>SADBL/55460/416.34</t>
+  </si>
+  <si>
+    <t>SHIVM/36449/524.25</t>
+  </si>
+  <si>
+    <t>NRIC/9583/1,264.79</t>
+  </si>
+  <si>
+    <t>SHIVM/52644/527.42</t>
+  </si>
+  <si>
+    <t>NRN/12620/2,035.51</t>
+  </si>
+  <si>
+    <t>BARUN/34015/508.16</t>
+  </si>
+  <si>
+    <t>SONA/34317/461.34</t>
+  </si>
+  <si>
+    <t>PRIN/16123/872.02</t>
+  </si>
+  <si>
+    <t>HIDCL/163566/306.34</t>
+  </si>
+  <si>
+    <t>KBL/205690/215.49</t>
+  </si>
+  <si>
+    <t>SHPC/36090/605.09</t>
+  </si>
+  <si>
+    <t>MEN/23885/579.77</t>
+  </si>
+  <si>
+    <t>NICA/34509/357.61</t>
+  </si>
+  <si>
+    <t>RADHI/78529/755.31</t>
+  </si>
+  <si>
+    <t>NGPL/97076/380.53</t>
+  </si>
+  <si>
+    <t>NRN/11693/2,079.90</t>
+  </si>
+  <si>
+    <t>BHL/99714/218.18</t>
+  </si>
+  <si>
+    <t>MEN/34930/583.89</t>
+  </si>
+  <si>
+    <t>SAHAS/177758/527.03</t>
+  </si>
+  <si>
+    <t>BPCL/70035/521.82</t>
+  </si>
+  <si>
+    <t>NABBC/15586/1,568.30</t>
+  </si>
+  <si>
+    <t>CORBL/13522/2,410.00</t>
+  </si>
+  <si>
+    <t>NGPL/81045/383.37</t>
+  </si>
+  <si>
+    <t>RADHI/78704/745.62</t>
+  </si>
+  <si>
+    <t>AHPC/101878/588.68</t>
+  </si>
+  <si>
+    <t>UMHL/42940/512.68</t>
+  </si>
+  <si>
+    <t>HURJA/75208/266.48</t>
+  </si>
+  <si>
+    <t>DORDI/52100/406.37</t>
+  </si>
+  <si>
+    <t>CHDC/50235/2,563.06</t>
+  </si>
+  <si>
+    <t>UPCL/238386/433.33</t>
+  </si>
+  <si>
+    <t>HIDCL/96548/304.79</t>
+  </si>
+  <si>
+    <t>SHL/37400/579.45</t>
+  </si>
+  <si>
+    <t>DORDI/44877/402.08</t>
+  </si>
+  <si>
+    <t>SBL/528679/292.80</t>
+  </si>
+  <si>
+    <t>EBL/152862/652.69</t>
+  </si>
+  <si>
+    <t>RADHI/93116/752.73</t>
+  </si>
+  <si>
+    <t>UPCL/117237/430.26</t>
+  </si>
+  <si>
+    <t>CBBL/37460/902.93</t>
+  </si>
+  <si>
+    <t>API/324894/302.99</t>
+  </si>
+  <si>
+    <t>HIDCL/257352/307.90</t>
+  </si>
+  <si>
+    <t>RADHI/80214/751.66</t>
+  </si>
+  <si>
+    <t>MEN/67112/587.30</t>
+  </si>
+  <si>
+    <t>AHPC/129574/590.97</t>
+  </si>
+  <si>
+    <t>GBIME/218107/239.59</t>
+  </si>
+  <si>
+    <t>RADHI/51791/757.39</t>
+  </si>
+  <si>
+    <t>NIFRA/106911/281.55</t>
+  </si>
+  <si>
+    <t>UPCL/54300/421.91</t>
+  </si>
+  <si>
+    <t>HDHPC/98161/213.84</t>
+  </si>
+  <si>
+    <t>SBI/171312/410.16</t>
+  </si>
+  <si>
+    <t>KBL/77850/212.22</t>
+  </si>
+  <si>
+    <t>SPIL/19550/822.42</t>
+  </si>
+  <si>
+    <t>JBBL/42396/336.41</t>
+  </si>
+  <si>
+    <t>BPCL/25051/527.73</t>
+  </si>
+  <si>
+    <t>MEN/12144/583.78</t>
+  </si>
+  <si>
+    <t>SHPC/8447/591.38</t>
+  </si>
+  <si>
+    <t>BHPL/4455/953.55</t>
+  </si>
+  <si>
+    <t>NRN/2058/2,061.36</t>
+  </si>
+  <si>
+    <t>BARUN/7536/516.96</t>
+  </si>
+  <si>
+    <t>BPCL/229005/531.53</t>
+  </si>
+  <si>
+    <t>SHIVM/79182/526.82</t>
+  </si>
+  <si>
+    <t>ULBSL/8973/3,357.90</t>
+  </si>
+  <si>
+    <t>CHDC/11145/2,530.89</t>
+  </si>
+  <si>
+    <t>HPPL/52438/512.89</t>
+  </si>
+  <si>
+    <t>NRN/70415/2,060.39</t>
+  </si>
+  <si>
+    <t>RADHI/157578/736.97</t>
+  </si>
+  <si>
+    <t>UPCL/249277/425.40</t>
+  </si>
+  <si>
+    <t>CHDC/14189/2,563.34</t>
+  </si>
+  <si>
+    <t>SPDL/39834/384.14</t>
+  </si>
+  <si>
+    <t>BPCL/84413/512.72</t>
+  </si>
+  <si>
+    <t>MEN/23743/592.37</t>
+  </si>
+  <si>
+    <t>SANIMA/44130/317.83</t>
+  </si>
+  <si>
+    <t>NGPL/26873/377.85</t>
+  </si>
+  <si>
+    <t>CHDC/3576/2,540.31</t>
+  </si>
+  <si>
+    <t>SAPDBL/114083/983.77</t>
+  </si>
+  <si>
+    <t>NMIC/14674/2,079.30</t>
+  </si>
+  <si>
+    <t>SINDU/28705/885.55</t>
+  </si>
+  <si>
+    <t>SHIVM/45752/527.90</t>
+  </si>
+  <si>
+    <t>SPDL/38945/389.51</t>
+  </si>
+  <si>
+    <t>GBIME/908369/239.18</t>
+  </si>
+  <si>
+    <t>AHPC/291776/595.44</t>
+  </si>
+  <si>
+    <t>AKPL/343309/260.67</t>
+  </si>
+  <si>
+    <t>MERO/110899/743.16</t>
+  </si>
+  <si>
+    <t>SHPC/89029/596.78</t>
+  </si>
+  <si>
+    <t>BPCL/96748/538.55</t>
+  </si>
+  <si>
+    <t>RFPL/63838/504.62</t>
+  </si>
+  <si>
+    <t>SPIL/29188/822.37</t>
+  </si>
+  <si>
+    <t>USLB/11537/1,948.85</t>
+  </si>
+  <si>
+    <t>NMFBS/18908/2,415.42</t>
+  </si>
+  <si>
+    <t>EBL/162572/651.63</t>
+  </si>
+  <si>
+    <t>PPCL/154414/342.16</t>
+  </si>
+  <si>
+    <t>MLBL/128271/393.56</t>
+  </si>
+  <si>
+    <t>SANIMA/122509/319.02</t>
+  </si>
+  <si>
+    <t>AKPL/149027/262.23</t>
+  </si>
+  <si>
+    <t>SHPC/727402/594.78</t>
+  </si>
+  <si>
+    <t>GBIME/187876/225.09</t>
+  </si>
+  <si>
+    <t>CZBIL/196301/215.78</t>
+  </si>
+  <si>
+    <t>NLIC/50059/758.79</t>
+  </si>
+  <si>
+    <t>LSL/136574/216.54</t>
+  </si>
+  <si>
+    <t>API/43641/302.73</t>
+  </si>
+  <si>
+    <t>HPPL/14125/526.27</t>
+  </si>
+  <si>
+    <t>HIDCL/20793/295.64</t>
+  </si>
+  <si>
+    <t>SHPC/10423/577.00</t>
+  </si>
+  <si>
+    <t>UPPER/27189/201.65</t>
+  </si>
+  <si>
+    <t>AHPC/251448/592.09</t>
+  </si>
+  <si>
+    <t>AKPL/93008/265.00</t>
+  </si>
+  <si>
+    <t>AKJCL/92390/433.03</t>
+  </si>
+  <si>
+    <t>CREST/7751/1,955.09</t>
+  </si>
+  <si>
+    <t>SPDL/35747/383.34</t>
+  </si>
+  <si>
+    <t>SHL/229671/569.36</t>
+  </si>
+  <si>
+    <t>SHPC/94310/586.89</t>
+  </si>
+  <si>
+    <t>AHPC/141976/597.85</t>
+  </si>
+  <si>
+    <t>SHIVM/72078/525.25</t>
+  </si>
+  <si>
+    <t>RIDI/74427/269.18</t>
+  </si>
+  <si>
+    <t>MEN/93521/582.65</t>
+  </si>
+  <si>
+    <t>SHPC/84411/593.44</t>
+  </si>
+  <si>
+    <t>RADHI/57992/746.35</t>
+  </si>
+  <si>
+    <t>NTC/34369/866.75</t>
+  </si>
+  <si>
+    <t>BHL/134440/218.42</t>
+  </si>
+  <si>
+    <t>RADHI/445377/755.56</t>
+  </si>
+  <si>
+    <t>SHL/67231/575.99</t>
+  </si>
+  <si>
+    <t>SHEL/90187/284.17</t>
+  </si>
+  <si>
+    <t>SPIL/23012/805.05</t>
+  </si>
+  <si>
+    <t>HURJA/60757/260.70</t>
+  </si>
+  <si>
+    <t>AHPC/133318/590.34</t>
+  </si>
+  <si>
+    <t>CHDC/9199/2,582.06</t>
+  </si>
+  <si>
+    <t>AKPL/54221/255.50</t>
+  </si>
+  <si>
+    <t>API/41237/304.47</t>
+  </si>
+  <si>
+    <t>BHL/43922/218.16</t>
+  </si>
+  <si>
+    <t>CHDC/12052/2,582.42</t>
+  </si>
+  <si>
+    <t>AKJCL/68352/421.94</t>
+  </si>
+  <si>
+    <t>AHPC/41014/588.63</t>
+  </si>
+  <si>
+    <t>BARUN/18811/486.95</t>
+  </si>
+  <si>
+    <t>RNLI/16797/509.32</t>
+  </si>
+  <si>
+    <t>NMFBS/11336/2,434.83</t>
+  </si>
+  <si>
+    <t>NMIC/5535/2,076.40</t>
+  </si>
+  <si>
+    <t>MEN/17353/597.78</t>
+  </si>
+  <si>
+    <t>SHPC/10355/599.35</t>
+  </si>
+  <si>
+    <t>ULBSL/2248/3,329.00</t>
+  </si>
+  <si>
+    <t>STC/13534/5,067.77</t>
+  </si>
+  <si>
+    <t>SADBL/30797/422.47</t>
+  </si>
+  <si>
+    <t>UPCL/27046/441.27</t>
+  </si>
+  <si>
+    <t>BARUN/21990/524.05</t>
+  </si>
+  <si>
+    <t>CBBL/10312/862.35</t>
+  </si>
+  <si>
+    <t>GMLI/179615/2,592.64</t>
+  </si>
+  <si>
+    <t>NRIC/249900/1,292.87</t>
+  </si>
+  <si>
+    <t>NMIC/54977/1,948.30</t>
+  </si>
+  <si>
+    <t>NLG/95805/833.24</t>
+  </si>
+  <si>
+    <t>HDL/19766/1,217.79</t>
+  </si>
+  <si>
+    <t>NGPL/112264/388.81</t>
+  </si>
+  <si>
+    <t>UPCL/90863/431.41</t>
+  </si>
+  <si>
+    <t>RADHI/49193/766.32</t>
+  </si>
+  <si>
+    <t>SMHL/42296/944.38</t>
+  </si>
+  <si>
+    <t>BEDC/43076/721.26</t>
+  </si>
+  <si>
+    <t>NGPL/187573/384.28</t>
+  </si>
+  <si>
+    <t>AHPC/134182/589.64</t>
+  </si>
+  <si>
+    <t>RADHI/33071/745.77</t>
+  </si>
+  <si>
+    <t>BARUN/49904/491.37</t>
+  </si>
+  <si>
+    <t>GHL/87271/253.47</t>
+  </si>
+  <si>
+    <t>KBL/1997893/214.79</t>
+  </si>
+  <si>
+    <t>NRN/174644/2,040.68</t>
+  </si>
+  <si>
+    <t>AHPC/794864/595.07</t>
+  </si>
+  <si>
+    <t>NGPL/415856/384.25</t>
+  </si>
+  <si>
+    <t>OHL/108721/949.46</t>
+  </si>
+  <si>
+    <t>NIFRA/75932/285.95</t>
+  </si>
+  <si>
+    <t>ALICL/28268/704.38</t>
+  </si>
+  <si>
+    <t>API/64092/302.75</t>
+  </si>
+  <si>
+    <t>NGPL/48317/384.07</t>
+  </si>
+  <si>
+    <t>SHIVM/24458/526.31</t>
+  </si>
+  <si>
+    <t>RADHI/146674/763.12</t>
+  </si>
+  <si>
+    <t>UPCL/164795/429.16</t>
+  </si>
+  <si>
+    <t>SHL/71938/568.21</t>
+  </si>
+  <si>
+    <t>LBBL/50310/474.65</t>
+  </si>
+  <si>
+    <t>SHPC/42161/582.79</t>
+  </si>
+  <si>
+    <t>BPCL/33450/561.40</t>
+  </si>
+  <si>
+    <t>CREST/5832/1,908.90</t>
+  </si>
+  <si>
+    <t>HIDCL/28439/306.20</t>
+  </si>
+  <si>
+    <t>NMIC/3976/2,034.30</t>
+  </si>
+  <si>
+    <t>UMHL/383512/506.29</t>
+  </si>
+  <si>
+    <t>RIDI/191208/269.67</t>
+  </si>
+  <si>
+    <t>BPCL/78619/543.28</t>
+  </si>
+  <si>
+    <t>AHPC/124134/600.96</t>
+  </si>
+  <si>
+    <t>ANLB/3990/5,389.84</t>
+  </si>
+  <si>
+    <t>RADHI/29514/753.98</t>
+  </si>
+  <si>
+    <t>OMPL/7630/1,831.61</t>
+  </si>
+  <si>
+    <t>AKPL/48118/263.46</t>
+  </si>
+  <si>
+    <t>SHL/22905/563.77</t>
+  </si>
+  <si>
+    <t>USLB/6013/1,930.13</t>
+  </si>
+  <si>
+    <t>BPCL/257379/528.72</t>
+  </si>
+  <si>
+    <t>CGH/100143/850.80</t>
+  </si>
+  <si>
+    <t>SHPC/79752/600.11</t>
+  </si>
+  <si>
+    <t>NRN/18716/2,060.10</t>
+  </si>
+  <si>
+    <t>BEDC/45597/744.81</t>
+  </si>
+  <si>
+    <t>SARBTM/83984/858.97</t>
+  </si>
+  <si>
+    <t>SANIMA/104667/318.78</t>
+  </si>
+  <si>
+    <t>PHCL/47464/597.10</t>
+  </si>
+  <si>
+    <t>NIFRA/103681/283.13</t>
+  </si>
+  <si>
+    <t>CHDC/38723/2,571.25</t>
+  </si>
+  <si>
+    <t>NRN/13532/2,050.05</t>
+  </si>
+  <si>
+    <t>UHEWA/35760/628.89</t>
+  </si>
+  <si>
+    <t>NGPL/63219/377.16</t>
+  </si>
+  <si>
+    <t>HIDCL/65110/297.26</t>
+  </si>
+  <si>
+    <t>RADHI/131398/770.38</t>
+  </si>
+  <si>
+    <t>HIDCL/77198/303.59</t>
+  </si>
+  <si>
+    <t>SHIVM/22923/535.81</t>
+  </si>
+  <si>
+    <t>HRL/11794/958.27</t>
+  </si>
+  <si>
+    <t>SHEL/26983/282.32</t>
+  </si>
+  <si>
+    <t>NGPL/148395/383.70</t>
+  </si>
+  <si>
+    <t>AHPC/103894/583.26</t>
+  </si>
+  <si>
+    <t>RIDI/69093/262.76</t>
+  </si>
+  <si>
+    <t>SHPC/15913/596.82</t>
+  </si>
+  <si>
+    <t>MLBL/24540/394.54</t>
+  </si>
+  <si>
+    <t>SHL/74881/563.37</t>
+  </si>
+  <si>
+    <t>HIDCL/82236/306.94</t>
+  </si>
+  <si>
+    <t>BPCL/37485/599.06</t>
+  </si>
+  <si>
+    <t>GLH/67661/278.85</t>
+  </si>
+  <si>
+    <t>SANIMA/53454/310.08</t>
+  </si>
+  <si>
+    <t>BPCL/73325/565.53</t>
+  </si>
+  <si>
+    <t>SHPC/53638/590.39</t>
+  </si>
+  <si>
+    <t>HPPL/33917/494.68</t>
+  </si>
+  <si>
+    <t>RADHI/16462/754.90</t>
+  </si>
+  <si>
+    <t>RADHI/69499/741.95</t>
+  </si>
+  <si>
+    <t>UPCL/94664/428.81</t>
+  </si>
+  <si>
+    <t>LBBL/78983/466.45</t>
+  </si>
+  <si>
+    <t>API/78511/305.81</t>
+  </si>
+  <si>
+    <t>CORBL/6536/2,314.74</t>
+  </si>
+  <si>
+    <t>CORBL/59755/2,296.51</t>
+  </si>
+  <si>
+    <t>GRDBL/30361/1,176.68</t>
+  </si>
+  <si>
+    <t>JOSHI/78401/423.70</t>
+  </si>
+  <si>
+    <t>NRN/12433/2,058.85</t>
+  </si>
+  <si>
+    <t>CHDC/9360/2,560.88</t>
+  </si>
+  <si>
+    <t>BHL/1400/211.96</t>
+  </si>
+  <si>
+    <t>SHPC/63630/576.33</t>
+  </si>
+  <si>
+    <t>SAPDBL/20122/1,008.87</t>
+  </si>
+  <si>
+    <t>BNHC/23521/518.72</t>
+  </si>
+  <si>
+    <t>SKBBL/15012/803.69</t>
+  </si>
+  <si>
+    <t>UPCL/30414/421.78</t>
+  </si>
+  <si>
+    <t>NRN/14351/2,071.40</t>
+  </si>
+  <si>
+    <t>RADHI/23064/751.31</t>
+  </si>
+  <si>
+    <t>API/45012/304.43</t>
+  </si>
+  <si>
+    <t>BHL/55520/215.50</t>
+  </si>
+  <si>
+    <t>BPCL/15470/579.77</t>
+  </si>
+  <si>
+    <t>SHIVM/11971/526.02</t>
+  </si>
+  <si>
+    <t>MEN/7486/577.51</t>
+  </si>
+  <si>
+    <t>BPCL/269750/564.04</t>
+  </si>
+  <si>
+    <t>RADHI/106820/770.75</t>
+  </si>
+  <si>
+    <t>UPCL/101600/427.21</t>
+  </si>
+  <si>
+    <t>CHDC/14098/2,553.56</t>
+  </si>
+  <si>
+    <t>SHPC/53593/593.70</t>
+  </si>
+  <si>
+    <t>NRN/2589/2,056.57</t>
+  </si>
+  <si>
+    <t>RADHI/6232/757.05</t>
+  </si>
+  <si>
+    <t>NGPL/10265/380.13</t>
+  </si>
+  <si>
+    <t>RNLI/6369/509.56</t>
+  </si>
+  <si>
+    <t>TRH/1100/948.00</t>
+  </si>
+  <si>
+    <t>AKJCL/4460/411.88</t>
+  </si>
+  <si>
+    <t>AHPC/2608/571.76</t>
+  </si>
+  <si>
+    <t>MEN/56630/584.50</t>
+  </si>
+  <si>
+    <t>NMLBBL/35723/661.47</t>
+  </si>
+  <si>
+    <t>RADHI/23868/760.42</t>
+  </si>
+  <si>
+    <t>NIFRA/56269/287.29</t>
+  </si>
+  <si>
+    <t>HRL/14886/967.00</t>
+  </si>
+  <si>
+    <t>UPCL/252631/424.51</t>
+  </si>
+  <si>
+    <t>NGPL/219998/391.51</t>
+  </si>
+  <si>
+    <t>SAHAS/62166/526.43</t>
+  </si>
+  <si>
+    <t>RIDI/102188/270.44</t>
+  </si>
+  <si>
+    <t>HRL/16982/982.04</t>
+  </si>
+  <si>
+    <t>NRN/17709/2,063.17</t>
+  </si>
+  <si>
+    <t>RADHI/39817/749.32</t>
+  </si>
+  <si>
+    <t>UMHL/23142/510.47</t>
+  </si>
+  <si>
+    <t>HRL/12128/957.17</t>
+  </si>
+  <si>
+    <t>RADHI/25156/757.82</t>
+  </si>
+  <si>
+    <t>HRL/18571/957.12</t>
+  </si>
+  <si>
+    <t>KPCL/18514/522.70</t>
+  </si>
+  <si>
+    <t>CGH/7390/872.73</t>
+  </si>
+  <si>
+    <t>SADBL/49231/422.33</t>
+  </si>
+  <si>
+    <t>HIDCL/62798/301.14</t>
+  </si>
+  <si>
+    <t>HDL/14525/1,216.24</t>
+  </si>
+  <si>
+    <t>KSBBL/34260/449.24</t>
+  </si>
+  <si>
+    <t>CZBIL/68811/214.42</t>
+  </si>
+  <si>
+    <t>NGPL/188297/381.05</t>
+  </si>
+  <si>
+    <t>SHL/81992/582.69</t>
+  </si>
+  <si>
+    <t>RADHI/55478/756.50</t>
+  </si>
+  <si>
+    <t>AHPC/68712/587.35</t>
+  </si>
+  <si>
+    <t>NRN/6666/2,078.15</t>
+  </si>
+  <si>
+    <t>CHDC/6217/2,564.38</t>
+  </si>
+  <si>
+    <t>UPCL/31242/418.80</t>
+  </si>
+  <si>
+    <t>NRIC/9567/1,283.84</t>
+  </si>
+  <si>
+    <t>RADHI/16263/751.77</t>
+  </si>
+  <si>
+    <t>SHPC/16539/591.50</t>
+  </si>
+  <si>
+    <t>RADHI/94763/751.07</t>
+  </si>
+  <si>
+    <t>RIDI/24200/269.73</t>
+  </si>
+  <si>
+    <t>HPPL/12297/510.10</t>
+  </si>
+  <si>
+    <t>UPCL/15960/417.17</t>
+  </si>
+  <si>
+    <t>NMIC/1916/2,068.14</t>
+  </si>
+  <si>
+    <t>SAPDBL/58064/988.42</t>
+  </si>
+  <si>
+    <t>CHDC/5491/2,518.60</t>
+  </si>
+  <si>
+    <t>CORBL/5210/2,578.93</t>
+  </si>
+  <si>
+    <t>NLG/12524/802.15</t>
+  </si>
+  <si>
+    <t>SHPC/13811/587.58</t>
+  </si>
+  <si>
+    <t>RADHI/28479/752.40</t>
+  </si>
+  <si>
+    <t>GBIME/87799/236.23</t>
+  </si>
+  <si>
+    <t>NGPL/20225/380.99</t>
+  </si>
+  <si>
+    <t>SHIVM/10225/525.77</t>
+  </si>
+  <si>
+    <t>HRL/3972/974.31</t>
+  </si>
+  <si>
+    <t>HBL/93145/230.84</t>
+  </si>
+  <si>
+    <t>SHL/12709/572.65</t>
+  </si>
+  <si>
+    <t>AHPC/15602/587.86</t>
+  </si>
+  <si>
+    <t>BARUN/5245/508.13</t>
+  </si>
+  <si>
+    <t>UPCL/67132/427.14</t>
+  </si>
+  <si>
+    <t>BPCL/32305/535.72</t>
+  </si>
+  <si>
+    <t>UNHPL/33858/336.58</t>
+  </si>
+  <si>
+    <t>HURJA/33600/264.04</t>
+  </si>
+  <si>
+    <t>AKPL/41269/260.77</t>
+  </si>
+  <si>
+    <t>HIDCL/179238/301.38</t>
+  </si>
+  <si>
+    <t>SHPC/19803/597.75</t>
+  </si>
+  <si>
+    <t>BPCL/16962/553.94</t>
+  </si>
+  <si>
+    <t>RADHI/12780/751.57</t>
+  </si>
+  <si>
+    <t>CHCL/11914/507.50</t>
+  </si>
+  <si>
+    <t>HEI/15674/582.63</t>
+  </si>
+  <si>
+    <t>SHPC/6910/592.48</t>
+  </si>
+  <si>
+    <t>ICFC/6110/616.11</t>
+  </si>
+  <si>
+    <t>SRLI/8751/405.83</t>
+  </si>
+  <si>
+    <t>RADHI/187305/760.88</t>
+  </si>
+  <si>
+    <t>MKHL/142541/730.51</t>
+  </si>
+  <si>
+    <t>UPCL/81171/422.40</t>
+  </si>
+  <si>
+    <t>PRIN/34648/867.00</t>
+  </si>
+  <si>
+    <t>BPCL/43375/522.29</t>
+  </si>
+  <si>
+    <t>UPCL/69391/442.92</t>
+  </si>
+  <si>
+    <t>NGPL/30773/387.19</t>
+  </si>
+  <si>
+    <t>RADHI/10025/761.35</t>
+  </si>
+  <si>
+    <t>NMIC/2640/2,166.84</t>
+  </si>
+  <si>
+    <t>NICA/17364/366.34</t>
+  </si>
+  <si>
+    <t>LBBL/168556/469.61</t>
+  </si>
+  <si>
+    <t>NICA/121914/365.05</t>
+  </si>
+  <si>
+    <t>SHL/65694/561.65</t>
+  </si>
+  <si>
+    <t>NRIC/22440/1,280.54</t>
+  </si>
+  <si>
+    <t>SHPC/38188/600.29</t>
+  </si>
+  <si>
+    <t>UPCL/31709/433.55</t>
+  </si>
+  <si>
+    <t>NRN/5807/2,043.42</t>
+  </si>
+  <si>
+    <t>SADBL/23810/423.36</t>
+  </si>
+  <si>
+    <t>SHPC/16681/590.94</t>
+  </si>
+  <si>
+    <t>NMIC/4008/2,082.93</t>
+  </si>
+  <si>
+    <t>RADHI/30457/741.78</t>
+  </si>
+  <si>
+    <t>NGPL/42738/384.56</t>
+  </si>
+  <si>
+    <t>API/43628/309.37</t>
+  </si>
+  <si>
+    <t>OMPL/7080/1,901.85</t>
+  </si>
+  <si>
+    <t>AHPC/45018/584.73</t>
+  </si>
+  <si>
+    <t>BPCL/25585/575.97</t>
+  </si>
+  <si>
+    <t>SHIVM/25230/536.05</t>
+  </si>
+  <si>
+    <t>UNHPL/35014/344.11</t>
+  </si>
+  <si>
+    <t>UPCL/22210/424.17</t>
+  </si>
+  <si>
+    <t>HPPL/13160/505.84</t>
+  </si>
+  <si>
+    <t>PHCL/112184/604.06</t>
+  </si>
+  <si>
+    <t>MLBL/60035/388.37</t>
+  </si>
+  <si>
+    <t>RADHI/20512/781.26</t>
+  </si>
+  <si>
+    <t>KSBBL/31631/452.73</t>
+  </si>
+  <si>
+    <t>LBBL/28098/453.18</t>
+  </si>
+  <si>
+    <t>CHDC/4265/2,576.84</t>
+  </si>
+  <si>
+    <t>RADHI/8657/763.30</t>
+  </si>
+  <si>
+    <t>AKPL/14500/274.51</t>
+  </si>
+  <si>
+    <t>RFPL/8705/475.82</t>
+  </si>
+  <si>
+    <t>NGPL/9450/390.08</t>
   </si>
 </sst>
 </file>
@@ -9773,11 +11091,1890 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001CC29C-638A-4E4E-829D-66241B93D88A}">
+  <dimension ref="A1:F93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3143</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3146</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3148</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3151</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3153</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3156</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3161</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3162</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3166</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3167</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3168</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3172</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3173</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2778</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3176</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3177</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3180</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3181</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3182</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3184</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3185</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3186</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3187</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3189</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3190</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3191</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3195</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3197</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3200</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3201</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3202</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3204</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3205</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3206</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3208</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3209</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3210</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3211</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3213</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2817</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3214</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3216</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3217</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3218</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3219</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3221</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3222</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3223</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3224</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3227</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3228</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3229</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3231</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3232</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3233</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3234</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3237</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3238</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3239</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3241</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3242</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3246</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3247</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3248</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3249</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3251</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3252</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3253</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3254</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3256</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3257</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3258</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3259</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3261</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3262</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3263</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3264</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3266</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3267</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3268</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3269</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3271</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3272</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3273</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3274</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3276</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3277</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3278</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3279</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3283</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3284</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3286</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3287</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3288</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3289</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3291</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3292</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3293</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3294</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3296</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3297</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3298</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3299</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3302</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3303</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3304</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3306</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3307</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3308</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3309</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3311</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3312</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3313</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3314</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3316</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3317</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3318</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3319</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3321</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3323</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3324</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3326</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3327</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3328</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3329</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3331</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3332</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3333</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3336</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3337</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3338</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3339</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3341</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3342</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3343</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3344</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3348</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3349</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3351</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3353</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3354</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3356</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3358</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3359</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3361</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3362</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3363</v>
+      </c>
+      <c r="E47" t="s">
+        <v>3364</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3366</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3367</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3368</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3369</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3372</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3373</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3374</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>288</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3376</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3377</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3378</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3379</v>
+      </c>
+      <c r="F50" t="s">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3382</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3383</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3384</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>300</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3386</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3387</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3388</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3389</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>306</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3392</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2986</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3393</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3394</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>312</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3396</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3397</v>
+      </c>
+      <c r="E54" t="s">
+        <v>3398</v>
+      </c>
+      <c r="F54" t="s">
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3400</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3401</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3402</v>
+      </c>
+      <c r="E55" t="s">
+        <v>3403</v>
+      </c>
+      <c r="F55" t="s">
+        <v>3404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3406</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3407</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3408</v>
+      </c>
+      <c r="F56" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>330</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3410</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3411</v>
+      </c>
+      <c r="E57" t="s">
+        <v>3412</v>
+      </c>
+      <c r="F57" t="s">
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>336</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3414</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3415</v>
+      </c>
+      <c r="D58" t="s">
+        <v>3416</v>
+      </c>
+      <c r="E58" t="s">
+        <v>3417</v>
+      </c>
+      <c r="F58" t="s">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>342</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3419</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3420</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3421</v>
+      </c>
+      <c r="E59" t="s">
+        <v>3422</v>
+      </c>
+      <c r="F59" t="s">
+        <v>3423</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>348</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3425</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3426</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3427</v>
+      </c>
+      <c r="F60" t="s">
+        <v>3428</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>354</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3429</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3430</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3431</v>
+      </c>
+      <c r="E61" t="s">
+        <v>3432</v>
+      </c>
+      <c r="F61" t="s">
+        <v>3433</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>360</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3434</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3435</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2188</v>
+      </c>
+      <c r="E62" t="s">
+        <v>3436</v>
+      </c>
+      <c r="F62" t="s">
+        <v>3437</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>366</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3438</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3439</v>
+      </c>
+      <c r="D63" t="s">
+        <v>3440</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3441</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3442</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>372</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3443</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3444</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3445</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3446</v>
+      </c>
+      <c r="F64" t="s">
+        <v>3447</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>378</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3036</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3448</v>
+      </c>
+      <c r="D65" t="s">
+        <v>381</v>
+      </c>
+      <c r="E65" t="s">
+        <v>2630</v>
+      </c>
+      <c r="F65" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3449</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3450</v>
+      </c>
+      <c r="D66" t="s">
+        <v>3451</v>
+      </c>
+      <c r="E66" t="s">
+        <v>3452</v>
+      </c>
+      <c r="F66" t="s">
+        <v>3453</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>390</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3454</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3455</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3456</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2210</v>
+      </c>
+      <c r="F67" t="s">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>396</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3458</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3046</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3459</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F68" t="s">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3461</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3462</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3463</v>
+      </c>
+      <c r="E69" t="s">
+        <v>3464</v>
+      </c>
+      <c r="F69" t="s">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>408</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3053</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3466</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3467</v>
+      </c>
+      <c r="E70" t="s">
+        <v>3468</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3469</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>414</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3470</v>
+      </c>
+      <c r="D71" t="s">
+        <v>3471</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3472</v>
+      </c>
+      <c r="F71" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>420</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3473</v>
+      </c>
+      <c r="C72" t="s">
+        <v>3474</v>
+      </c>
+      <c r="D72" t="s">
+        <v>3475</v>
+      </c>
+      <c r="E72" t="s">
+        <v>3476</v>
+      </c>
+      <c r="F72" t="s">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>426</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3478</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3479</v>
+      </c>
+      <c r="D73" t="s">
+        <v>3480</v>
+      </c>
+      <c r="E73" t="s">
+        <v>3481</v>
+      </c>
+      <c r="F73" t="s">
+        <v>3482</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>432</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3483</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3484</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2662</v>
+      </c>
+      <c r="E74" t="s">
+        <v>3485</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>438</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3487</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3488</v>
+      </c>
+      <c r="D75" t="s">
+        <v>3489</v>
+      </c>
+      <c r="E75" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F75" t="s">
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>444</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3491</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3492</v>
+      </c>
+      <c r="D76" t="s">
+        <v>3493</v>
+      </c>
+      <c r="E76" t="s">
+        <v>3494</v>
+      </c>
+      <c r="F76" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>450</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C77" t="s">
+        <v>3497</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E77" t="s">
+        <v>3499</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>456</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3502</v>
+      </c>
+      <c r="D78" t="s">
+        <v>3503</v>
+      </c>
+      <c r="E78" t="s">
+        <v>3504</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>462</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3506</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3507</v>
+      </c>
+      <c r="D79" t="s">
+        <v>3508</v>
+      </c>
+      <c r="E79" t="s">
+        <v>3509</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>468</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3511</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3512</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3513</v>
+      </c>
+      <c r="E80" t="s">
+        <v>3514</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>474</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C81" t="s">
+        <v>3517</v>
+      </c>
+      <c r="D81" t="s">
+        <v>3518</v>
+      </c>
+      <c r="E81" t="s">
+        <v>3519</v>
+      </c>
+      <c r="F81" t="s">
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>480</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3521</v>
+      </c>
+      <c r="C82" t="s">
+        <v>3522</v>
+      </c>
+      <c r="D82" t="s">
+        <v>3523</v>
+      </c>
+      <c r="E82" t="s">
+        <v>3524</v>
+      </c>
+      <c r="F82" t="s">
+        <v>3098</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>486</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3525</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3526</v>
+      </c>
+      <c r="D83" t="s">
+        <v>3527</v>
+      </c>
+      <c r="E83" t="s">
+        <v>3528</v>
+      </c>
+      <c r="F83" t="s">
+        <v>3529</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>492</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3530</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3531</v>
+      </c>
+      <c r="D84" t="s">
+        <v>3532</v>
+      </c>
+      <c r="E84" t="s">
+        <v>3533</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>498</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3535</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3536</v>
+      </c>
+      <c r="D85" t="s">
+        <v>3537</v>
+      </c>
+      <c r="E85" t="s">
+        <v>2709</v>
+      </c>
+      <c r="F85" t="s">
+        <v>3538</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>504</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3539</v>
+      </c>
+      <c r="C86" t="s">
+        <v>3540</v>
+      </c>
+      <c r="D86" t="s">
+        <v>3541</v>
+      </c>
+      <c r="E86" t="s">
+        <v>3542</v>
+      </c>
+      <c r="F86" t="s">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>510</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3544</v>
+      </c>
+      <c r="C87" t="s">
+        <v>3545</v>
+      </c>
+      <c r="D87" t="s">
+        <v>3546</v>
+      </c>
+      <c r="E87" t="s">
+        <v>3547</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>516</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3549</v>
+      </c>
+      <c r="C88" t="s">
+        <v>3550</v>
+      </c>
+      <c r="D88" t="s">
+        <v>3551</v>
+      </c>
+      <c r="E88" t="s">
+        <v>3552</v>
+      </c>
+      <c r="F88" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>522</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C89" t="s">
+        <v>3555</v>
+      </c>
+      <c r="D89" t="s">
+        <v>3556</v>
+      </c>
+      <c r="E89" t="s">
+        <v>3557</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3558</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>528</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3559</v>
+      </c>
+      <c r="C90" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D90" t="s">
+        <v>3561</v>
+      </c>
+      <c r="E90" t="s">
+        <v>3562</v>
+      </c>
+      <c r="F90" t="s">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>534</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3565</v>
+      </c>
+      <c r="D91" t="s">
+        <v>3566</v>
+      </c>
+      <c r="E91" t="s">
+        <v>3567</v>
+      </c>
+      <c r="F91" t="s">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>540</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3569</v>
+      </c>
+      <c r="C92" t="s">
+        <v>3570</v>
+      </c>
+      <c r="D92" t="s">
+        <v>3571</v>
+      </c>
+      <c r="E92" t="s">
+        <v>3572</v>
+      </c>
+      <c r="F92" t="s">
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>546</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3574</v>
+      </c>
+      <c r="C93" t="s">
+        <v>3575</v>
+      </c>
+      <c r="D93" t="s">
+        <v>3576</v>
+      </c>
+      <c r="E93" t="s">
+        <v>3577</v>
+      </c>
+      <c r="F93" t="s">
+        <v>3578</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C0AFDA-3FBB-41A3-BA62-46EDDC71FB68}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11654,7 +14851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676205A0-C5FF-4AEC-B10B-18D60F60A28C}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -13536,7 +16733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FC7E8D-1DE3-4DBF-BC92-6657EED87D10}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -15419,7 +18616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EEF453-2C93-48DA-92A9-F02917F02C21}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -17301,7 +20498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3009EEF-D0A3-4418-BB02-D308992E6389}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -19181,7 +22378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62503B16-5D5E-43EB-8EDC-28C65E9BFBAD}">
   <dimension ref="A1:F93"/>
   <sheetViews>
@@ -21061,7 +24258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F93"/>
   <sheetViews>

</xml_diff>